<commit_message>
v1.2 Publish & Upload feature is reviewed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{3A9422EA-D275-4626-854E-AFA48F80ECC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1B44F85A-1D02-4024-BE9E-31AEBB1DFBA9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="4005" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -61,79 +62,75 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Ahmed Abuzaid</t>
-  </si>
-  <si>
     <t>v1.0</t>
   </si>
   <si>
     <t>intial version</t>
   </si>
   <si>
-    <t>LH_REVIEW_SRS_LOGIN_001</t>
+    <t>SRS ID</t>
   </si>
   <si>
     <t>SRS-LOGIN-001</t>
   </si>
   <si>
-    <t>SRS_ID</t>
+    <t>LH-REVIEW-SRS-001</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-002</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-003</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-004</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-005</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-006</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-007</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-008</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-009</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the requirement is vague regarding the type of identifier allowed in the login form. Please clarify whether the system accepts only email address or both email and username for login. Additionally, specify any validation rules for the email field (e.g., format, required field). This helps ensureproper implementation and avoids ambiguity during development and testing.  </t>
+  </si>
+  <si>
+    <t>Ahmed Abozaid</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>SRS-LOGIN-002</t>
   </si>
   <si>
-    <t>SRS-LOGIN-003</t>
-  </si>
-  <si>
-    <t>SRS-LOGIN-004</t>
-  </si>
-  <si>
-    <t>Hala Eldaly</t>
-  </si>
-  <si>
-    <t>The requirement is vague regarding the type of identifier allowed in the login 
-form. Please clarify whether the system accepts only email addresses or both 
-email and usernames for login. Additionally, specify any validation rules for 
-the email field (e.g., format, required field). This helps ensure proper implementation and avoids ambiguity during development and testing.</t>
-  </si>
-  <si>
-    <t>No comments</t>
-  </si>
-  <si>
-    <t>Consider clarifying whether user feedback on failed logins
-(e.g., email vs. password issue) is intentionally generic for security reason</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>not applicable</t>
-  </si>
-  <si>
-    <t>Ensure that you update the login form to
- handle both email and username options 
-if applicable, and implement proper email 
-validation (e.g., format, required field) to
- prevent issues during login and testing.</t>
-  </si>
-  <si>
-    <t>Please confirm whether the user feedback 
-for failed logins should remain generic
- (e.g., 'Invalid credentials') for security
- reasons, or if more specific messages
- (e.g., 'Incorrect email' or 'Incorrect password') 
-are acceptable.</t>
-  </si>
-  <si>
-    <t>v1.1</t>
+    <t>Please confirm whether the user feedback for failed logins should remain generic (e.g., 'Invalid credentials') for security reasons, or if more specific messages (e.g., 'Incorrect email' or 'Incorrect password') are acceptable.</t>
+  </si>
+  <si>
+    <t>Ensure that you update the login form to handle both email and username options if applicable, and implement proper email validation (e.g., format, required field) to prevent issues during login and testing.</t>
+  </si>
+  <si>
+    <t>Consider clarifying whether user feedback on failed logins (e.g., email vs. password issue) is intentionally generic for security reason</t>
   </si>
   <si>
     <t>SRS-ID-001</t>
   </si>
   <si>
-    <t>LH_REVIEW_SRS_ID CONSTRAINS_001</t>
-  </si>
-  <si>
     <t>The SRS requirement does not explicitly mention that the User ID must be unique, as stated in the CRS.</t>
   </si>
   <si>
@@ -141,13 +138,82 @@
   </si>
   <si>
     <t>Added review comments under ID_CONSTRAINTS_REVIEWS, updated the version, and renamed the file to align with the naming convention defined in the project plan.</t>
+  </si>
+  <si>
+    <t>SRS-PUB-001</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>v 1.1</t>
+  </si>
+  <si>
+    <t>The SRS does not mention what happens after clicking each button.</t>
+  </si>
+  <si>
+    <t>Try to clarify that each button will direct the user to a related interface. Recommendation: add "each leading to the respective submission interface"</t>
+  </si>
+  <si>
+    <t>SRS-PUB-002</t>
+  </si>
+  <si>
+    <t>Try to make the requirement a bit clearer so it’s easier to understand for everyone, especially those who are not deeply technical.</t>
+  </si>
+  <si>
+    <t>Recommendation: The system shall validate video file size before upload and reject files exceeding 100MB, with the message: "Max size: 100MB."</t>
+  </si>
+  <si>
+    <t>SRS-PUB-003</t>
+  </si>
+  <si>
+    <t>The same as the above</t>
+  </si>
+  <si>
+    <t>Recommendation:The system shall validate audio file size before upload and reject files exceeding 20MB, with the message: "Max size: 20MB."</t>
+  </si>
+  <si>
+    <t>SRS-PUB-004</t>
+  </si>
+  <si>
+    <t>What does the word 'dynamically' refer to? Runtime or on submission? Needs to be clearer</t>
+  </si>
+  <si>
+    <t>Recommendation: The system shall count words in articles in real-time and prevent submission if the article exceeds 1000 words.</t>
+  </si>
+  <si>
+    <t>SRS-PUB-005</t>
+  </si>
+  <si>
+    <t>Consider replacing “.MP4” with “MP4 format” to improve readability and make it clearer.</t>
+  </si>
+  <si>
+    <t>Recommendation: The system shall allow only .mp4 video files to be uploaded. If an unsupported format (e.g., .avi) is selected, display: "Only MP4 format is allowed."</t>
+  </si>
+  <si>
+    <t>SRS-PUB-006</t>
+  </si>
+  <si>
+    <t>The same as the above ".MP3" with "MP3 format".</t>
+  </si>
+  <si>
+    <t>Recommendation: The system shall allow only .mp3 audio files to be uploaded. If another format (e.g., .wav) is selected, display the message: "Only MP3 format is allowed."</t>
+  </si>
+  <si>
+    <t>Reviewed Publish and upload feature</t>
+  </si>
+  <si>
+    <t>14-Ape-25</t>
+  </si>
+  <si>
+    <t>v1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,21 +257,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,12 +297,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6F8F9"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -267,6 +338,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -306,68 +403,55 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -383,73 +467,93 @@
     <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -727,266 +831,466 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="86.5703125" customWidth="1"/>
-    <col min="7" max="7" width="56" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="94.85546875" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="18.75">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18.75">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="23" customFormat="1" ht="68.25" customHeight="1">
+      <c r="A2" s="5">
+        <f>DATE(2025,4,13)</f>
+        <v>45760</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45">
+      <c r="A3" s="28">
+        <f>DATE(2025,4,13)</f>
+        <v>45760</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="131.25">
-      <c r="A2" s="27">
-        <v>45760</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="32" t="s">
+      <c r="C3" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30">
+      <c r="A4" s="5">
+        <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
+        <v>45761</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30">
+      <c r="A5" s="6">
+        <f t="shared" si="0"/>
+        <v>45761</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="43"/>
+    </row>
+    <row r="6" spans="1:11" ht="30">
+      <c r="A6" s="5">
+        <f t="shared" si="0"/>
+        <v>45761</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="43"/>
+    </row>
+    <row r="7" spans="1:11" ht="30">
+      <c r="A7" s="6">
+        <f t="shared" si="0"/>
+        <v>45761</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="C7" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
+      <c r="A8" s="5">
+        <f t="shared" si="0"/>
+        <v>45761</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="28"/>
-      <c r="B3" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="14" t="s">
+      <c r="C8" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="35.25" customHeight="1">
+      <c r="A9" s="6">
+        <f t="shared" si="0"/>
+        <v>45761</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="22"/>
-    </row>
-    <row r="4" spans="1:10" ht="112.5">
-      <c r="A4" s="28"/>
-      <c r="B4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="15" t="s">
+      <c r="C9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45">
+      <c r="A10" s="5">
+        <f t="shared" si="0"/>
+        <v>45761</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="C10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18.75">
-      <c r="A5" s="29"/>
-      <c r="B5" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:10" ht="75">
-      <c r="A6" s="24">
-        <v>45761</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="D9" s="17"/>
+      <c r="I10" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="2"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="5"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="E2:E6"/>
-  </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="D2" s="38">
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="112.5">
-      <c r="A3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="13">
+    <row r="3" spans="1:4" ht="75">
+      <c r="A3" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="41">
         <v>45761</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.3 Reviewed the System Constrains and the Registration
LH_SRS_REGISTERATION_Review_011
LH_SRS_SYSTEMCONSTRAINS_Review_16
Added the review points on both system constrains and registration in the SRS
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3A9422EA-D275-4626-854E-AFA48F80ECC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1B44F85A-1D02-4024-BE9E-31AEBB1DFBA9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCB2FDD-D1AD-4AD6-9163-F0F0C746AD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -16,12 +16,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -203,17 +214,91 @@
     <t>Reviewed Publish and upload feature</t>
   </si>
   <si>
-    <t>14-Ape-25</t>
-  </si>
-  <si>
     <t>v1.2</t>
+  </si>
+  <si>
+    <t>v1.3</t>
+  </si>
+  <si>
+    <t>Mahmoud Abdelmageed</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-010</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-011</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-012</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-013</t>
+  </si>
+  <si>
+    <t>SRS-REG-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The message is very big to be shown inside the password field box(inline) </t>
+  </si>
+  <si>
+    <t>Recommendation: The message should be shown in a bigger area like next to the password field or in a popup</t>
+  </si>
+  <si>
+    <t>SRS-REG-005</t>
+  </si>
+  <si>
+    <t>Recommendation: The description should be :The system shall ensure that the username is unique. If a duplicate username is detected, an error message shall be displayed, saying : This username is already used</t>
+  </si>
+  <si>
+    <t>the description has some language mistakes that should be corrected for better understanding of the requirement</t>
+  </si>
+  <si>
+    <t>SRS-REG-006</t>
+  </si>
+  <si>
+    <t>Recommendation: The description should be :The system shall validate email to be unique and if not an error message should appear saying : This E-mail is already used</t>
+  </si>
+  <si>
+    <t>SRS-SYS-001</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The CRS did not state that the PC and Web application should have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>identical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> feature sets</t>
+    </r>
+  </si>
+  <si>
+    <t>Recommendation: Rephrase the description to avoid implying that the PC and web applications must have identical feature sets, as differences between platforms make this challenging to implement</t>
+  </si>
+  <si>
+    <t>Reviewed Registration and System Constrains</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +348,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,8 +419,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -342,19 +454,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -422,36 +521,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -467,55 +560,55 @@
     <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyAlignment="1">
@@ -539,18 +632,27 @@
     <xf numFmtId="15" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -832,387 +934,657 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="G3" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="94.85546875" customWidth="1"/>
-    <col min="7" max="7" width="76.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="77.77734375" customWidth="1"/>
+    <col min="7" max="7" width="76.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18.75">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="23" customFormat="1" ht="68.25" customHeight="1">
-      <c r="A2" s="5">
+    <row r="2" spans="1:11" s="19" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="45">
-      <c r="A3" s="28">
+      <c r="I2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="24">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30">
-      <c r="A4" s="5">
-        <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
+      <c r="I3" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <f t="shared" ref="A4:B19" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30">
-      <c r="A5" s="6">
+      <c r="I4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="43"/>
-    </row>
-    <row r="6" spans="1:11" ht="30">
-      <c r="A6" s="5">
+      <c r="I5" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="39"/>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="43"/>
-    </row>
-    <row r="7" spans="1:11" ht="30">
-      <c r="A7" s="6">
+      <c r="I6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="39"/>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="5">
+      <c r="I7" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="35.25" customHeight="1">
-      <c r="A9" s="6">
+      <c r="I8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45">
-      <c r="A10" s="5">
+      <c r="I9" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="5"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="I10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <f>DATE(2025,4,17)</f>
+        <v>45764</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="41">
+        <f t="shared" ref="A12:A21" si="1">DATE(2025,4,17)</f>
+        <v>45764</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <f t="shared" si="1"/>
+        <v>45764</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="41">
+        <f t="shared" si="1"/>
+        <v>45764</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1222,77 +1594,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="34">
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:4" ht="74.400000000000006" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="37">
         <v>45761</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="13">
+        <v>45761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>60</v>
+      <c r="B5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="13">
+        <v>45764</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.4 Reviewed Admin Constraints
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCB2FDD-D1AD-4AD6-9163-F0F0C746AD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A596EDCC-C36D-4DCB-9327-65BAE5385B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,8 +23,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -293,12 +291,76 @@
   <si>
     <t>Reviewed Registration and System Constrains</t>
   </si>
+  <si>
+    <t>LH-REVIEW-SRS-014</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omar Sherif </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spelling Error </t>
+  </si>
+  <si>
+    <t>Header Consistency</t>
+  </si>
+  <si>
+    <t>The header "ADMIN Constrain" should be updated to "ADMIN Constraints" for grammatical correctness.</t>
+  </si>
+  <si>
+    <t>Inconsistent Naming Convention</t>
+  </si>
+  <si>
+    <t>SRS-ADM-001</t>
+  </si>
+  <si>
+    <t>SRS-ADM-002</t>
+  </si>
+  <si>
+    <t>The word "admains". It should be corrected to "admins" in both constraints.</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-016</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed Admin Constraints </t>
+  </si>
+  <si>
+    <r>
+      <t>In the first column, the ID uses "CONSTRAINS" instead of "CONSTRAIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S". It should be fixed to maintain naming consistency </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +427,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -538,13 +607,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -561,18 +623,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -584,9 +634,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,13 +641,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -632,9 +673,6 @@
     <xf numFmtId="15" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,15 +682,102 @@
     <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -936,152 +1061,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="77.77734375" customWidth="1"/>
-    <col min="7" max="7" width="76.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="41" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="41" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="41" customWidth="1"/>
+    <col min="6" max="6" width="77.77734375" style="53" customWidth="1"/>
+    <col min="7" max="7" width="76.33203125" style="48" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" style="41" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" style="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="19" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="12" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="21" t="s">
+      <c r="I2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="24">
+      <c r="A3" s="16">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:B19" si="0">DATE(2025,4,14)</f>
+        <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="21" t="s">
+      <c r="I4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1090,99 +1215,99 @@
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="39"/>
+      <c r="I5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="39"/>
+      <c r="I6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="28"/>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="30" t="s">
+      <c r="I7" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1191,31 +1316,31 @@
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="21" t="s">
+      <c r="I8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1224,31 +1349,31 @@
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="30" t="s">
+      <c r="I9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="20" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1257,31 +1382,31 @@
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="21" t="s">
+      <c r="I10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1290,64 +1415,64 @@
         <f>DATE(2025,4,17)</f>
         <v>45764</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="30" t="s">
+      <c r="I11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="41">
-        <f t="shared" ref="A12:A21" si="1">DATE(2025,4,17)</f>
+      <c r="A12" s="30">
+        <f t="shared" ref="A12:A16" si="1">DATE(2025,4,17)</f>
         <v>45764</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="11" t="s">
         <v>70</v>
       </c>
       <c r="D12" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="21" t="s">
+      <c r="I12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1356,227 +1481,291 @@
         <f t="shared" si="1"/>
         <v>45764</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="30" t="s">
+      <c r="I13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="A14" s="30">
         <f t="shared" si="1"/>
         <v>45764</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="I14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36">
+        <f>DATE(2025,4,18)</f>
+        <v>45765</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="37">
+        <f>A17</f>
+        <v>45765</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="38">
+        <f>DATE(2025,4,18)</f>
+        <v>45765</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -1594,10 +1783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1609,73 +1798,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="24">
         <v>45760</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="74.400000000000006" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="27">
         <v>45761</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="10">
         <v>45761</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>45764</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="10">
+        <v>45765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.5 update owner status after modify SRS
update owner status of some SRSs after modify SRS file depending on reviewers comments
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A596EDCC-C36D-4DCB-9327-65BAE5385B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -292,43 +282,43 @@
     <t>Reviewed Registration and System Constrains</t>
   </si>
   <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
     <t>LH-REVIEW-SRS-014</t>
   </si>
   <si>
+    <t>SRS-ADM-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omar Sherif </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spelling Error </t>
+  </si>
+  <si>
+    <t>The word "admains". It should be corrected to "admins" in both constraints.</t>
+  </si>
+  <si>
     <t>LH-REVIEW-SRS-015</t>
   </si>
   <si>
-    <t xml:space="preserve">Omar Sherif </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spelling Error </t>
-  </si>
-  <si>
     <t>Header Consistency</t>
   </si>
   <si>
     <t>The header "ADMIN Constrain" should be updated to "ADMIN Constraints" for grammatical correctness.</t>
   </si>
   <si>
+    <t>LH-REVIEW-SRS-016</t>
+  </si>
+  <si>
+    <t>SRS-ADM-002</t>
+  </si>
+  <si>
     <t>Inconsistent Naming Convention</t>
-  </si>
-  <si>
-    <t>SRS-ADM-001</t>
-  </si>
-  <si>
-    <t>SRS-ADM-002</t>
-  </si>
-  <si>
-    <t>The word "admains". It should be corrected to "admins" in both constraints.</t>
-  </si>
-  <si>
-    <t>LH-REVIEW-SRS-016</t>
-  </si>
-  <si>
-    <t>v1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewed Admin Constraints </t>
   </si>
   <si>
     <r>
@@ -355,12 +345,18 @@
       <t xml:space="preserve">S". It should be fixed to maintain naming consistency </t>
     </r>
   </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed Admin Constraints </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,6 +603,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -623,6 +626,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -634,6 +649,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -641,7 +659,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -652,9 +676,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -673,6 +694,9 @@
     <xf numFmtId="15" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,15 +706,23 @@
     <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -706,63 +738,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -775,8 +759,14 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1058,722 +1048,719 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="41" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" style="41" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="41" customWidth="1"/>
-    <col min="6" max="6" width="77.77734375" style="53" customWidth="1"/>
-    <col min="7" max="7" width="76.33203125" style="48" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" style="41" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.88671875" style="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="19" customFormat="1" ht="75">
       <c r="A2" s="4">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+    </row>
+    <row r="3" spans="1:11" ht="45">
+      <c r="A3" s="24">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="28"/>
-    </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K6" s="38"/>
+    </row>
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="F8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" ht="35.25" customHeight="1">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" ht="30">
       <c r="A11" s="5">
         <f>DATE(2025,4,17)</f>
         <v>45764</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="G11" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="20" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="45">
+      <c r="A12" s="40">
+        <f t="shared" ref="A12:A14" si="1">DATE(2025,4,17)</f>
+        <v>45764</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
-        <f t="shared" ref="A12:A16" si="1">DATE(2025,4,17)</f>
-        <v>45764</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>45764</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="55" t="s">
+      <c r="G13" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="30">
+    </row>
+    <row r="14" spans="1:11" ht="45">
+      <c r="A14" s="40">
         <f t="shared" si="1"/>
         <v>45764</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="14" t="s">
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="50">
+        <v>45765</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="56" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36">
-        <f>DATE(2025,4,18)</f>
+    <row r="16" spans="1:11" ht="30">
+      <c r="A16" s="51">
         <v>45765</v>
       </c>
-      <c r="B15" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="34" t="s">
+      <c r="B16" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="35" t="s">
+      <c r="C16" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="32" t="s">
+      <c r="F16" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H16" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="56" t="s">
+      <c r="I16" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="58" t="s">
+    </row>
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" s="52">
+        <v>45765</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="37">
-        <f>A17</f>
-        <v>45765</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="59" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" s="59" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="38">
-        <f>DATE(2025,4,18)</f>
-        <v>45765</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="5"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1782,102 +1769,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="78.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="20.25">
+      <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:4" ht="18.75">
+      <c r="A2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="33">
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="74.400000000000006" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:4" ht="75">
+      <c r="A3" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="36">
         <v>45761</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" ht="18.75">
+      <c r="A4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="13">
         <v>45761</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" ht="37.5">
+      <c r="A5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="13">
         <v>45764</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="10">
+    <row r="6" spans="1:4" ht="18.75">
+      <c r="A6" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="62">
         <v>45765</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.5 closed publish and upload reviews
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A7EFE6-0AC2-4A36-8D34-9342C644AD68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -357,11 +358,17 @@
   <si>
     <t>Close reviewer verification for Login and ID_Constraints</t>
   </si>
+  <si>
+    <t>v1.6</t>
+  </si>
+  <si>
+    <t>Close reviewer verification for Publish and upload feature</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -1054,11 +1061,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1236,7 +1243,7 @@
         <v>80</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="K5" s="38"/>
     </row>
@@ -1270,7 +1277,7 @@
         <v>80</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="K6" s="38"/>
     </row>
@@ -1304,7 +1311,7 @@
         <v>80</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
@@ -1337,7 +1344,7 @@
         <v>80</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="35.25" customHeight="1">
@@ -1370,7 +1377,7 @@
         <v>80</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45">
@@ -1403,7 +1410,7 @@
         <v>80</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30">
@@ -1763,10 +1770,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1775,11 +1782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1888,6 +1895,20 @@
         <v>45765</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="18.75">
+      <c r="A8" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="33">
+        <v>45765</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.7 changed the reviewer status of registration and system contstrains
LH_SRS_REGISTERATION_Review_011
LH_SRS_SYSTEMCONSTRAINS_Review_16
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C263751-31AE-4688-B94C-2DFD97C57970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FCA186-451B-4F48-B02B-1C4C4510682C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t>Close reviewer verification for Publish and upload feature</t>
+  </si>
+  <si>
+    <t>v1.7</t>
+  </si>
+  <si>
+    <t>Changed reviewer verification for Registration and System Constrains</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -1779,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1905,6 +1911,20 @@
         <v>45765</v>
       </c>
     </row>
+    <row r="9" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="33">
+        <v>45766</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.8 Changed reviewer verification for Admin Constrains
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FCA186-451B-4F48-B02B-1C4C4510682C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7440303A-5DC6-45B0-90EA-B7C092A3EFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -23,8 +23,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -380,6 +378,12 @@
   </si>
   <si>
     <t>Changed reviewer verification for Registration and System Constrains</t>
+  </si>
+  <si>
+    <t>v1.8</t>
+  </si>
+  <si>
+    <t>Changed reviewer verification for Admin Constrains</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,7 +1580,7 @@
         <v>80</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1608,7 +1612,7 @@
         <v>80</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1640,7 +1644,7 @@
         <v>80</v>
       </c>
       <c r="J17" s="49" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1785,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1925,6 +1929,20 @@
         <v>45766</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="33">
+        <v>45766</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.9  Changed reviewer verification for Navigation
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7440303A-5DC6-45B0-90EA-B7C092A3EFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E39E430-C199-4795-B479-BC29842C97A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -384,6 +384,39 @@
   </si>
   <si>
     <t>Changed reviewer verification for Admin Constrains</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-017</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-018</t>
+  </si>
+  <si>
+    <t>SRS-NAV-001</t>
+  </si>
+  <si>
+    <t>SRS-NAV-002</t>
+  </si>
+  <si>
+    <t>v 1.2</t>
+  </si>
+  <si>
+    <t>Explicitly list the 4 categories in the SRS</t>
+  </si>
+  <si>
+    <t>The SRS does not define the 4 predefined content categories (e.g., names like ‘Home’, ‘Products’).</t>
+  </si>
+  <si>
+    <t>The SRS lacks testable criteria for dropdown interactions (e.g., hover vs. click)</t>
+  </si>
+  <si>
+    <t>Add acceptance criteria: Dropdowns must open on hover or Click (on desktop)</t>
+  </si>
+  <si>
+    <t>v1.9</t>
+  </si>
+  <si>
+    <t>Changed reviewer verification for Navigation</t>
   </si>
 </sst>
 </file>
@@ -620,7 +653,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -787,6 +820,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1070,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23:J24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1647,28 +1690,69 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+    <row r="18" spans="1:10" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="58">
+        <v>45765</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="60" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
+      <c r="A19" s="5">
+        <v>45765</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="26"/>
@@ -1789,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1943,6 +2027,20 @@
         <v>45766</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="33">
+        <v>45767</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v2.0 reviewed publish article with no comments
LH_SRS_PUBLISHARTICLE_Review
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E39E430-C199-4795-B479-BC29842C97A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68020C2-A822-4021-BD4E-89DD23CFF524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -417,6 +417,30 @@
   </si>
   <si>
     <t>Changed reviewer verification for Navigation</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>Reviewed publish video</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-019</t>
+  </si>
+  <si>
+    <t>SRS-PUBART</t>
+  </si>
+  <si>
+    <t>v2.3</t>
+  </si>
+  <si>
+    <t>No review Comments</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Gehad ashry</t>
   </si>
 </sst>
 </file>
@@ -653,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -830,6 +854,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1113,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="G8" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,15 +1782,36 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="A20" s="62">
+        <v>45785</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="26" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
@@ -1873,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2041,6 +2089,20 @@
         <v>45767</v>
       </c>
     </row>
+    <row r="12" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="33">
+        <v>45785</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v2.3 Reviewed publish Video & Admin Home  SRS
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAB72F5-6CCB-4C27-A23D-3866F0FEFE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -19,8 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="146">
   <si>
     <t>date</t>
   </si>
@@ -239,7 +243,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">The CRS did not state that the PC and Web application should have </t>
@@ -250,7 +254,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>identical</t>
@@ -260,7 +264,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> feature sets</t>
@@ -308,7 +312,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>In the first column, the ID uses "CONSTRAINS" instead of "CONSTRAIN</t>
@@ -318,7 +322,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>T</t>
@@ -328,7 +332,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">S". It should be fixed to maintain naming consistency </t>
@@ -499,18 +503,42 @@
   <si>
     <t>Reviewed publish Audio</t>
   </si>
+  <si>
+    <t>LH-REVIEW-SRS-023</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-024</t>
+  </si>
+  <si>
+    <t>CRS IDs use LH-CRS-PUBLISHVIDEO-XXX, but SRS IDs use LH-SRS-PUBVID-XXX.</t>
+  </si>
+  <si>
+    <t>Align SRS IDs with CRS format (e.g., LH-SRS-PUBLISHVIDEO-XXX).</t>
+  </si>
+  <si>
+    <t>Mahmoud</t>
+  </si>
+  <si>
+    <t>SRS-PUBLISHVIDEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed publish Video &amp; Admin Home </t>
+  </si>
+  <si>
+    <t>SRS-ADMIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use namig by the name of the feature ADMIN Constrains </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naming like LH-SRS-DELETEPOST what is deletpost </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="29">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,31 +547,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="16"/>
       <color theme="0"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="0"/>
       <name val="Roboto"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="15"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -551,122 +592,21 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -674,61 +614,24 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -755,7 +658,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,204 +670,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
+        <bgColor theme="4" tint="0.79995117038483843"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor theme="4" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <bgColor theme="4" tint="0.79995117038483843"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1054,286 +777,47 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1343,16 +827,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="26" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1361,7 +845,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1385,7 +869,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1401,10 +885,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1412,7 +896,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1442,16 +926,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1478,62 +962,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1791,33 +1235,33 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="G17" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.4380952380952" style="15" customWidth="1"/>
-    <col min="2" max="2" width="19.552380952381" customWidth="1"/>
-    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="22.8857142857143" customWidth="1"/>
-    <col min="5" max="5" width="11.8857142857143" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="85" customWidth="1"/>
-    <col min="7" max="7" width="76.3333333333333" customWidth="1"/>
-    <col min="8" max="8" width="19.1047619047619" customWidth="1"/>
-    <col min="9" max="9" width="21.6666666666667" customWidth="1"/>
-    <col min="10" max="10" width="30.8857142857143" customWidth="1"/>
+    <col min="7" max="7" width="76.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" ht="18.75" spans="1:10">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="18">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="1" ht="75" spans="1:10">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="57.6">
       <c r="A2" s="18">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1882,7 +1326,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" ht="45" spans="1:10">
+    <row r="3" spans="1:11" ht="43.2">
       <c r="A3" s="22">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1915,7 +1359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" ht="30" spans="1:10">
+    <row r="4" spans="1:11" ht="28.8">
       <c r="A4" s="18">
         <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
@@ -1948,7 +1392,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:11">
+    <row r="5" spans="1:11" ht="28.8">
       <c r="A5" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1982,7 +1426,7 @@
       </c>
       <c r="K5" s="59"/>
     </row>
-    <row r="6" ht="30" spans="1:11">
+    <row r="6" spans="1:11" ht="28.8">
       <c r="A6" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2016,7 +1460,7 @@
       </c>
       <c r="K6" s="59"/>
     </row>
-    <row r="7" ht="30" spans="1:10">
+    <row r="7" spans="1:11" ht="28.8">
       <c r="A7" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2049,7 +1493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" ht="30" spans="1:10">
+    <row r="8" spans="1:11" ht="28.8">
       <c r="A8" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2082,7 +1526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" ht="35.25" customHeight="1" spans="1:10">
+    <row r="9" spans="1:11" ht="35.25" customHeight="1">
       <c r="A9" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2115,7 +1559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" ht="45" spans="1:10">
+    <row r="10" spans="1:11" ht="28.8">
       <c r="A10" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2148,7 +1592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="1:10">
+    <row r="11" spans="1:11" ht="28.8">
       <c r="A11" s="30">
         <f>DATE(2025,4,17)</f>
         <v>45764</v>
@@ -2181,7 +1625,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" ht="45" spans="1:10">
+    <row r="12" spans="1:11" ht="43.2">
       <c r="A12" s="36">
         <f t="shared" ref="A12:A14" si="1">DATE(2025,4,17)</f>
         <v>45764</v>
@@ -2214,7 +1658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" ht="30" spans="1:10">
+    <row r="13" spans="1:11" ht="28.8">
       <c r="A13" s="30">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -2247,7 +1691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" ht="45" spans="1:10">
+    <row r="14" spans="1:11" ht="43.2">
       <c r="A14" s="36">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -2280,7 +1724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="41">
         <v>45765</v>
       </c>
@@ -2312,7 +1756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" ht="30" spans="1:10">
+    <row r="16" spans="1:11" ht="28.8">
       <c r="A16" s="36">
         <v>45765</v>
       </c>
@@ -2344,7 +1788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" ht="30" spans="1:10">
+    <row r="17" spans="1:10" ht="28.8">
       <c r="A17" s="30">
         <v>45765</v>
       </c>
@@ -2376,7 +1820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="1" spans="1:10">
+    <row r="18" spans="1:10" s="14" customFormat="1">
       <c r="A18" s="51">
         <v>45765</v>
       </c>
@@ -2504,7 +1948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" ht="75" spans="1:10">
+    <row r="22" spans="1:10" ht="72">
       <c r="A22" s="53">
         <v>45786</v>
       </c>
@@ -2558,7 +2002,7 @@
       <c r="G23" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="63" t="s">
         <v>16</v>
       </c>
       <c r="I23" s="25" t="s">
@@ -2568,27 +2012,73 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="3:10">
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-    </row>
-    <row r="25" spans="3:10">
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-    </row>
-    <row r="26" spans="3:10">
+    <row r="24" spans="1:10">
+      <c r="A24" s="53">
+        <v>45786</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="53">
+        <v>45786</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="53"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
@@ -2598,7 +2088,7 @@
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
     </row>
-    <row r="27" spans="3:10">
+    <row r="27" spans="1:10">
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
@@ -2608,7 +2098,7 @@
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
     </row>
-    <row r="28" spans="3:10">
+    <row r="28" spans="1:10">
       <c r="C28" s="25"/>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -2618,7 +2108,7 @@
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
     </row>
-    <row r="29" spans="3:10">
+    <row r="29" spans="1:10">
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
@@ -2629,37 +2119,36 @@
       <c r="J29" s="25"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.1047619047619" customWidth="1"/>
-    <col min="2" max="2" width="33.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="78.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="23.8857142857143" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" spans="1:4">
+    <row r="1" spans="1:4" ht="21">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -2673,7 +2162,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:4">
+    <row r="2" spans="1:4" ht="18.600000000000001">
       <c r="A2" s="3" t="s">
         <v>111</v>
       </c>
@@ -2687,7 +2176,7 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="3" ht="75" spans="1:4">
+    <row r="3" spans="1:4" ht="74.400000000000006">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -2701,7 +2190,7 @@
         <v>45761</v>
       </c>
     </row>
-    <row r="4" ht="18.75" spans="1:4">
+    <row r="4" spans="1:4" ht="18.600000000000001">
       <c r="A4" s="9" t="s">
         <v>114</v>
       </c>
@@ -2715,7 +2204,7 @@
         <v>45761</v>
       </c>
     </row>
-    <row r="5" ht="37.5" spans="1:4">
+    <row r="5" spans="1:4" ht="18.600000000000001">
       <c r="A5" s="9" t="s">
         <v>116</v>
       </c>
@@ -2729,7 +2218,7 @@
         <v>45764</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="1:4">
+    <row r="6" spans="1:4" ht="18.600000000000001">
       <c r="A6" s="9" t="s">
         <v>118</v>
       </c>
@@ -2743,7 +2232,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="7" ht="18.75" spans="1:4">
+    <row r="7" spans="1:4" ht="18.600000000000001">
       <c r="A7" s="3" t="s">
         <v>120</v>
       </c>
@@ -2757,7 +2246,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="8" ht="18.75" spans="1:4">
+    <row r="8" spans="1:4" ht="18.600000000000001">
       <c r="A8" s="3" t="s">
         <v>122</v>
       </c>
@@ -2771,7 +2260,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="9" ht="37.5" spans="1:4">
+    <row r="9" spans="1:4" ht="37.200000000000003">
       <c r="A9" s="3" t="s">
         <v>124</v>
       </c>
@@ -2785,7 +2274,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="10" ht="18.75" spans="1:4">
+    <row r="10" spans="1:4" ht="18.600000000000001">
       <c r="A10" s="3" t="s">
         <v>126</v>
       </c>
@@ -2799,7 +2288,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="11" ht="18.75" spans="1:4">
+    <row r="11" spans="1:4" ht="18.600000000000001">
       <c r="A11" s="3" t="s">
         <v>128</v>
       </c>
@@ -2813,7 +2302,7 @@
         <v>45767</v>
       </c>
     </row>
-    <row r="12" ht="18.75" spans="1:4">
+    <row r="12" spans="1:4" ht="18.600000000000001">
       <c r="A12" s="3" t="s">
         <v>130</v>
       </c>
@@ -2827,7 +2316,7 @@
         <v>45785</v>
       </c>
     </row>
-    <row r="13" ht="18.75" spans="1:4">
+    <row r="13" spans="1:4" ht="18.600000000000001">
       <c r="A13" s="3" t="s">
         <v>132</v>
       </c>
@@ -2841,7 +2330,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="14" ht="18.75" spans="1:4">
+    <row r="14" spans="1:4" ht="18.600000000000001">
       <c r="A14" s="3" t="s">
         <v>134</v>
       </c>
@@ -2855,8 +2344,22 @@
         <v>45786</v>
       </c>
     </row>
+    <row r="15" spans="1:4" ht="18.600000000000001">
+      <c r="A15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="5">
+        <v>45786</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2.4 reviewed registration SRS
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\new_repo\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAB72F5-6CCB-4C27-A23D-3866F0FEFE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="159">
   <si>
     <t>date</t>
   </si>
@@ -402,9 +401,6 @@
 but the record must stop automatically..</t>
   </si>
   <si>
-    <t>my recommendation is to eliminate the LH-SRS-PUBLISHAUDIO-007, or remove the part that mention the automatic stop of the recording to solve this conflict.</t>
-  </si>
-  <si>
     <t>LH-REVIEW-SRS-022</t>
   </si>
   <si>
@@ -532,12 +528,55 @@
   </si>
   <si>
     <t xml:space="preserve">Naming like LH-SRS-DELETEPOST what is deletpost </t>
+  </si>
+  <si>
+    <t>my recommendation is to eliminate the LH-SRS-PUBLISHAUDIO-007, or remove
+ the part that mention the automatic stop of the recording to solve this conflict.</t>
+  </si>
+  <si>
+    <t>v2.4</t>
+  </si>
+  <si>
+    <t>Ahme Abuzaid</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-025</t>
+  </si>
+  <si>
+    <t>SRS-REGISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make all the error messages as generic message  </t>
+  </si>
+  <si>
+    <t>you make a different error message for each error</t>
+  </si>
+  <si>
+    <t>Omar sherif</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-001</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-026</t>
+  </si>
+  <si>
+    <t>this srs is vague</t>
+  </si>
+  <si>
+    <t>so it can be more specific and mention the component of the registration form like "the registration form consist of user name field,email field,password field and register button"</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>Reviewed Registration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -782,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -962,8 +1001,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1240,28 +1288,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="G17" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="85" customWidth="1"/>
-    <col min="7" max="7" width="76.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="10" max="10" width="30.88671875" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="18">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="18.75">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="13" customFormat="1" ht="57.6">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="75">
       <c r="A2" s="18">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1326,7 +1374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.2">
+    <row r="3" spans="1:11" ht="45">
       <c r="A3" s="22">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1359,7 +1407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="18">
         <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
@@ -1392,7 +1440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8">
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1426,7 +1474,7 @@
       </c>
       <c r="K5" s="59"/>
     </row>
-    <row r="6" spans="1:11" ht="28.8">
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1460,7 +1508,7 @@
       </c>
       <c r="K6" s="59"/>
     </row>
-    <row r="7" spans="1:11" ht="28.8">
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1493,7 +1541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8">
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1559,7 +1607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8">
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1592,7 +1640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8">
+    <row r="11" spans="1:11" ht="30">
       <c r="A11" s="30">
         <f>DATE(2025,4,17)</f>
         <v>45764</v>
@@ -1625,7 +1673,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43.2">
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="36">
         <f t="shared" ref="A12:A14" si="1">DATE(2025,4,17)</f>
         <v>45764</v>
@@ -1658,7 +1706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8">
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="30">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -1691,7 +1739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="43.2">
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="36">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -1756,7 +1804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="36">
         <v>45765</v>
       </c>
@@ -1788,7 +1836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="28.8">
+    <row r="17" spans="1:10" ht="30">
       <c r="A17" s="30">
         <v>45765</v>
       </c>
@@ -1948,183 +1996,229 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="72">
-      <c r="A22" s="53">
+    <row r="22" spans="1:10" ht="75">
+      <c r="A22" s="63">
         <v>45786</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="50" t="s">
+      <c r="F22" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="63">
+        <v>45786</v>
+      </c>
+      <c r="B23" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="C23" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I23" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J22" s="25" t="s">
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="63">
+        <v>45786</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="I24" s="57" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="53">
+      <c r="J24" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="63">
         <v>45786</v>
       </c>
-      <c r="B23" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="25" t="s">
+      <c r="B25" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="63" t="s">
+      <c r="F25" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="H25" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I25" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J25" s="57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="53">
+    <row r="26" spans="1:10">
+      <c r="A26" s="63">
         <v>45786</v>
       </c>
-      <c r="B24" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="63" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="G24" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="H24" s="63" t="s">
-        <v>140</v>
-      </c>
-      <c r="I24" s="25" t="s">
+      <c r="B26" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" t="s">
+        <v>151</v>
+      </c>
+      <c r="G26" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="H26" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="I26" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="J26" s="57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="53">
+    <row r="27" spans="1:10" ht="45">
+      <c r="A27" s="63">
         <v>45786</v>
       </c>
-      <c r="B25" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>143</v>
-      </c>
-      <c r="D25" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="63" t="s">
-        <v>145</v>
-      </c>
-      <c r="G25" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="H25" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="25" t="s">
+      <c r="B27" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="G27" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="H27" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="I27" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="25" t="s">
+      <c r="J27" s="57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="53"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-    </row>
     <row r="28" spans="1:10">
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="A29" s="60"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2133,50 +2227,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="78.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="18.75">
+      <c r="A2" s="3" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.600000000000001">
-      <c r="A2" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="74.400000000000006">
+    <row r="3" spans="1:4" ht="75">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -2184,167 +2278,167 @@
         <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="8">
         <v>45761</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001">
+    <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="11">
         <v>45761</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.600000000000001">
+    <row r="5" spans="1:4" ht="18.75">
       <c r="A5" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="11">
         <v>45764</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.600000000000001">
+    <row r="6" spans="1:4" ht="18.75">
       <c r="A6" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="11">
         <v>45765</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.600000000000001">
+    <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="5">
         <v>45765</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.600000000000001">
+    <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="5">
         <v>45765</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.200000000000003">
+    <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="5">
         <v>45766</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.600000000000001">
+    <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="5">
         <v>45766</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.600000000000001">
+    <row r="11" spans="1:4" ht="18.75">
       <c r="A11" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="5">
         <v>45767</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.600000000000001">
+    <row r="12" spans="1:4" ht="18.75">
       <c r="A12" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" s="5">
         <v>45785</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.600000000000001">
+    <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D13" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.600000000000001">
+    <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18.600000000000001">
+    <row r="15" spans="1:4" ht="18.75">
       <c r="A15" s="3" t="s">
         <v>93</v>
       </c>
@@ -2352,9 +2446,23 @@
         <v>72</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D15" s="5">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75">
+      <c r="A16" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="5">
         <v>45786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2.5 Reviewed CATEGORIES & LOGIN features
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\new_repo\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\hhh\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="180">
   <si>
     <t>date</t>
   </si>
@@ -572,12 +572,80 @@
   <si>
     <t>Reviewed Registration</t>
   </si>
+  <si>
+    <t>Reviewed CATEGORIES &amp; LOGIN features</t>
+  </si>
+  <si>
+    <t>v2.5</t>
+  </si>
+  <si>
+    <t>LH-SRS-CATEGORIES-007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clearly state the exact location where notifications will appear (e.g., Home Page banner, notification panel, or popup).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The SRS does not specify where the notifications will be shown in the UI. </t>
+  </si>
+  <si>
+    <t>Omar Shreif</t>
+  </si>
+  <si>
+    <t>LH-SRS-CATEGORIES-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify the exact redirection behavior, including whether it’s a full page reload, new tab/window, modal, or SPA routing.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The redirection method after selecting a publishing option is unclear (e.g., new page, new tab, modal, or in-page routing). </t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-027</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split this into two clear requirements: one for validating the email format, and another for checking if the user is registered.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The requirement merges email format validation and registration status check in one sentence, which may cause confusion. </t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-028</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify the salting approach more clearly or refer to a standard (e.g., per-user unique salt, random-generated salt).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The phrase “simple salting mechanism” is vague and may be interpreted differently by developers. </t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-029</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarify that plain-text passwords must not be stored in the database, logs, or transmitted over the network.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The phrase “at any stage” may raise ambiguity during input handling or temporary memory use. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,6 +733,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -821,7 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -971,9 +1045,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1012,6 +1083,57 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="11" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="11" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1289,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A20" zoomScale="50" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1337,7 +1459,7 @@
       <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1367,10 +1489,10 @@
       <c r="H2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="55" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1400,10 +1522,10 @@
       <c r="H3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="58" t="s">
+      <c r="I3" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="57" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1433,10 +1555,10 @@
       <c r="H4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="56" t="s">
+      <c r="I4" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="55" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1466,13 +1588,13 @@
       <c r="H5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="59"/>
+      <c r="I5" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="58"/>
     </row>
     <row r="6" spans="1:11" ht="30">
       <c r="A6" s="18">
@@ -1500,13 +1622,13 @@
       <c r="H6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="59"/>
+      <c r="I6" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="58"/>
     </row>
     <row r="7" spans="1:11" ht="30">
       <c r="A7" s="30">
@@ -1534,10 +1656,10 @@
       <c r="H7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="58" t="s">
+      <c r="I7" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="57" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1567,10 +1689,10 @@
       <c r="H8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="56" t="s">
+      <c r="I8" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="55" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1600,10 +1722,10 @@
       <c r="H9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="58" t="s">
+      <c r="I9" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="57" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1633,10 +1755,10 @@
       <c r="H10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="56" t="s">
+      <c r="I10" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="55" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1666,10 +1788,10 @@
       <c r="H11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="58" t="s">
+      <c r="I11" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="57" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1699,10 +1821,10 @@
       <c r="H12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="56" t="s">
+      <c r="I12" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="55" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1732,10 +1854,10 @@
       <c r="H13" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="58" t="s">
+      <c r="I13" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="57" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1765,10 +1887,10 @@
       <c r="H14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="56" t="s">
+      <c r="I14" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="55" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1797,10 +1919,10 @@
       <c r="H15" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="61" t="s">
+      <c r="I15" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="60" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1893,10 +2015,10 @@
       <c r="H18" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="62" t="s">
+      <c r="I18" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="62" t="s">
+      <c r="J18" s="61" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1932,35 +2054,35 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="53">
+    <row r="20" spans="1:10" s="81" customFormat="1">
+      <c r="A20" s="82">
         <v>45785</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="25" t="s">
+      <c r="I20" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="84" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1996,221 +2118,357 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="75">
-      <c r="A22" s="63">
+    <row r="22" spans="1:10" s="81" customFormat="1" ht="75">
+      <c r="A22" s="77">
         <v>45786</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="57" t="s">
+      <c r="D22" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="60" t="s">
+      <c r="G22" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="H22" s="57" t="s">
+      <c r="H22" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="57" t="s">
+      <c r="I22" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="79" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="63">
+      <c r="A23" s="62">
         <v>45786</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="57" t="s">
+      <c r="D23" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="57" t="s">
+      <c r="F23" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="G23" s="57" t="s">
+      <c r="G23" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="H23" s="65" t="s">
+      <c r="H23" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="57" t="s">
+      <c r="I23" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="56" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="63">
+    <row r="24" spans="1:10" s="81" customFormat="1">
+      <c r="A24" s="77">
         <v>45786</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="65" t="s">
+      <c r="E24" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="65" t="s">
+      <c r="F24" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="G24" s="65" t="s">
+      <c r="G24" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="H24" s="65" t="s">
+      <c r="H24" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="I24" s="57" t="s">
+      <c r="I24" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="57" t="s">
+      <c r="J24" s="79" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="63">
+      <c r="A25" s="62">
         <v>45786</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E25" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="65" t="s">
+      <c r="F25" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="G25" s="65" t="s">
+      <c r="G25" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="H25" s="65" t="s">
+      <c r="H25" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="57" t="s">
+      <c r="I25" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="57" t="s">
+      <c r="J25" s="56" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="63">
+    <row r="26" spans="1:10" s="81" customFormat="1">
+      <c r="A26" s="77">
         <v>45786</v>
       </c>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="D26" s="57" t="s">
+      <c r="D26" s="79" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="65" t="s">
+      <c r="E26" s="79" t="s">
         <v>146</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="81" t="s">
         <v>151</v>
       </c>
-      <c r="G26" s="57" t="s">
+      <c r="G26" s="79" t="s">
         <v>150</v>
       </c>
-      <c r="H26" s="57" t="s">
+      <c r="H26" s="79" t="s">
         <v>152</v>
       </c>
-      <c r="I26" s="57" t="s">
+      <c r="I26" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="57" t="s">
+      <c r="J26" s="79" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="45">
-      <c r="A27" s="63">
+      <c r="A27" s="62">
         <v>45786</v>
       </c>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="59" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="D27" s="57" t="s">
+      <c r="D27" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="F27" s="66" t="s">
+      <c r="F27" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="G27" s="64" t="s">
+      <c r="G27" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="H27" s="57" t="s">
+      <c r="H27" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="I27" s="57" t="s">
+      <c r="I27" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="J27" s="57" t="s">
+      <c r="J27" s="56" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="60"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="60"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
+    <row r="28" spans="1:10" s="70" customFormat="1" ht="60">
+      <c r="A28" s="66">
+        <v>45786</v>
+      </c>
+      <c r="B28" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="H28" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="I28" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="76" customFormat="1" ht="60">
+      <c r="A29" s="71">
+        <v>45786</v>
+      </c>
+      <c r="B29" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="H29" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="I29" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J29" s="75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="81" customFormat="1" ht="60">
+      <c r="A30" s="77">
+        <v>45786</v>
+      </c>
+      <c r="B30" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="79" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="G30" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="79" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="76" customFormat="1" ht="90">
+      <c r="A31" s="71">
+        <v>45786</v>
+      </c>
+      <c r="B31" s="72" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="G31" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="81" customFormat="1" ht="60">
+      <c r="A32" s="77">
+        <v>45786</v>
+      </c>
+      <c r="B32" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="80" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="79" t="s">
+        <v>179</v>
+      </c>
+      <c r="H32" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="J32" s="79" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -2228,10 +2486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2466,6 +2724,20 @@
         <v>45786</v>
       </c>
     </row>
+    <row r="17" spans="1:4" ht="18.75">
+      <c r="A17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="5">
+        <v>45786</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v2.7 Reviewed DELETEUSER feature
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\hhh\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -19,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="187">
   <si>
     <t>date</t>
   </si>
@@ -239,7 +242,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">The CRS did not state that the PC and Web application should have </t>
@@ -250,7 +253,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>identical</t>
@@ -260,7 +263,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> feature sets</t>
@@ -308,7 +311,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>In the first column, the ID uses "CONSTRAINS" instead of "CONSTRAIN</t>
@@ -318,7 +321,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>T</t>
@@ -328,7 +331,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">S". It should be fixed to maintain naming consistency </t>
@@ -398,47 +401,143 @@
 but the record must stop automatically..</t>
   </si>
   <si>
+    <t>LH-REVIEW-SRS-022</t>
+  </si>
+  <si>
+    <t>SRS-PUBLISHAUDIO-008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CRS did not mention anything related to a live timer, it will be static and after recording the evaluation of the record length will be executed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">please remove the part of "Live timer" </t>
+  </si>
+  <si>
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Updated section</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>intial version</t>
+  </si>
+  <si>
+    <t>Added review comments under ID_CONSTRAINTS_REVIEWS, updated the version, and renamed the file to align with the naming convention defined in the project plan.</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>Reviewed Publish and upload feature</t>
+  </si>
+  <si>
+    <t>v1.3</t>
+  </si>
+  <si>
+    <t>Reviewed Registration and System Constrains</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed Admin Constraints </t>
+  </si>
+  <si>
+    <t>v1.5</t>
+  </si>
+  <si>
+    <t>Close reviewer verification for Login and ID_Constraints</t>
+  </si>
+  <si>
+    <t>v1.6</t>
+  </si>
+  <si>
+    <t>Close reviewer verification for Publish and upload feature</t>
+  </si>
+  <si>
+    <t>v1.7</t>
+  </si>
+  <si>
+    <t>Changed reviewer verification for Registration and System Constrains</t>
+  </si>
+  <si>
+    <t>v1.8</t>
+  </si>
+  <si>
+    <t>Changed reviewer verification for Admin Constrains</t>
+  </si>
+  <si>
+    <t>v1.9</t>
+  </si>
+  <si>
+    <t>Changed reviewer verification for Navigation</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>Reviewed publish video</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>Reviewed Delete Post</t>
+  </si>
+  <si>
+    <t>v2.2</t>
+  </si>
+  <si>
+    <t>Reviewed publish Audio</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-023</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-024</t>
+  </si>
+  <si>
+    <t>CRS IDs use LH-CRS-PUBLISHVIDEO-XXX, but SRS IDs use LH-SRS-PUBVID-XXX.</t>
+  </si>
+  <si>
+    <t>Align SRS IDs with CRS format (e.g., LH-SRS-PUBLISHVIDEO-XXX).</t>
+  </si>
+  <si>
+    <t>Mahmoud</t>
+  </si>
+  <si>
+    <t>SRS-PUBLISHVIDEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed publish Video &amp; Admin Home </t>
+  </si>
+  <si>
+    <t>SRS-ADMIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use namig by the name of the feature ADMIN Constrains </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naming like LH-SRS-DELETEPOST what is deletpost </t>
+  </si>
+  <si>
     <t>my recommendation is to eliminate the LH-SRS-PUBLISHAUDIO-007, or remove
  the part that mention the automatic stop of the recording to solve this conflict.</t>
   </si>
   <si>
-    <t>LH-REVIEW-SRS-022</t>
-  </si>
-  <si>
-    <t>SRS-PUBLISHAUDIO-008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The CRS did not mention anything related to a live timer, it will be static and after recording the evaluation of the record length will be executed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">please remove the part of "Live timer" </t>
-  </si>
-  <si>
-    <t>LH-REVIEW-SRS-023</t>
-  </si>
-  <si>
-    <t>SRS-PUBLISHVIDEO</t>
-  </si>
-  <si>
-    <t>CRS IDs use LH-CRS-PUBLISHVIDEO-XXX, but SRS IDs use LH-SRS-PUBVID-XXX.</t>
-  </si>
-  <si>
-    <t>Align SRS IDs with CRS format (e.g., LH-SRS-PUBLISHVIDEO-XXX).</t>
-  </si>
-  <si>
-    <t>Mahmoud</t>
-  </si>
-  <si>
-    <t>LH-REVIEW-SRS-024</t>
-  </si>
-  <si>
-    <t>SRS-ADMIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naming like LH-SRS-DELETEPOST what is deletpost </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use namig by the name of the feature ADMIN Constrains </t>
+    <t>v2.4</t>
+  </si>
+  <si>
+    <t>Ahme Abuzaid</t>
   </si>
   <si>
     <t>LH-REVIEW-SRS-025</t>
@@ -447,189 +546,127 @@
     <t>SRS-REGISTRATION</t>
   </si>
   <si>
-    <t>Ahme Abuzaid</t>
-  </si>
-  <si>
-    <t>v2.4</t>
+    <t xml:space="preserve">make all the error messages as generic message  </t>
   </si>
   <si>
     <t>you make a different error message for each error</t>
   </si>
   <si>
-    <t xml:space="preserve">make all the error messages as generic message  </t>
-  </si>
-  <si>
     <t>Omar sherif</t>
   </si>
   <si>
+    <t>LH-SRS-REG-001</t>
+  </si>
+  <si>
     <t>LH-REVIEW-SRS-026</t>
   </si>
   <si>
-    <t>LH-SRS-REG-001</t>
-  </si>
-  <si>
     <t>this srs is vague</t>
   </si>
   <si>
     <t>so it can be more specific and mention the component of the registration form like "the registration form consist of user name field,email field,password field and register button"</t>
   </si>
   <si>
-    <t>Version number</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Updated section</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>v1.0</t>
-  </si>
-  <si>
-    <t>intial version</t>
-  </si>
-  <si>
-    <t>Added review comments under ID_CONSTRAINTS_REVIEWS, updated the version, and renamed the file to align with the naming convention defined in the project plan.</t>
-  </si>
-  <si>
-    <t>v1.2</t>
-  </si>
-  <si>
-    <t>Reviewed Publish and upload feature</t>
-  </si>
-  <si>
-    <t>v1.3</t>
-  </si>
-  <si>
-    <t>Reviewed Registration and System Constrains</t>
-  </si>
-  <si>
-    <t>v1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewed Admin Constraints </t>
-  </si>
-  <si>
-    <t>v1.5</t>
-  </si>
-  <si>
-    <t>Close reviewer verification for Login and ID_Constraints</t>
-  </si>
-  <si>
-    <t>v1.6</t>
-  </si>
-  <si>
-    <t>Close reviewer verification for Publish and upload feature</t>
-  </si>
-  <si>
-    <t>v1.7</t>
-  </si>
-  <si>
-    <t>Changed reviewer verification for Registration and System Constrains</t>
-  </si>
-  <si>
-    <t>v1.8</t>
-  </si>
-  <si>
-    <t>Changed reviewer verification for Admin Constrains</t>
-  </si>
-  <si>
-    <t>v1.9</t>
-  </si>
-  <si>
-    <t>Changed reviewer verification for Navigation</t>
-  </si>
-  <si>
-    <t>v2.0</t>
-  </si>
-  <si>
-    <t>Reviewed publish video</t>
-  </si>
-  <si>
-    <t>v2.1</t>
-  </si>
-  <si>
-    <t>Reviewed Delete Post</t>
-  </si>
-  <si>
-    <t>v2.2</t>
-  </si>
-  <si>
-    <t>Reviewed publish Audio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewed publish Video &amp; Admin Home </t>
-  </si>
-  <si>
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
     <t>Reviewed Registration</t>
   </si>
   <si>
+    <t>Reviewed CATEGORIES &amp; LOGIN features</t>
+  </si>
+  <si>
     <t>v2.5</t>
   </si>
   <si>
+    <t>LH-SRS-CATEGORIES-007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clearly state the exact location where notifications will appear (e.g., Home Page banner, notification panel, or popup).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The SRS does not specify where the notifications will be shown in the UI. </t>
+  </si>
+  <si>
+    <t>Omar Shreif</t>
+  </si>
+  <si>
+    <t>LH-SRS-CATEGORIES-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify the exact redirection behavior, including whether it’s a full page reload, new tab/window, modal, or SPA routing.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The redirection method after selecting a publishing option is unclear (e.g., new page, new tab, modal, or in-page routing). </t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-027</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split this into two clear requirements: one for validating the email format, and another for checking if the user is registered.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The requirement merges email format validation and registration status check in one sentence, which may cause confusion. </t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-028</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify the salting approach more clearly or refer to a standard (e.g., per-user unique salt, random-generated salt).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The phrase “simple salting mechanism” is vague and may be interpreted differently by developers. </t>
+  </si>
+  <si>
+    <t>LH-REVIEW-SRS-029</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarify that plain-text passwords must not be stored in the database, logs, or transmitted over the network.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The phrase “at any stage” may raise ambiguity during input handling or temporary memory use. </t>
+  </si>
+  <si>
     <t>Close reviewer verification</t>
+  </si>
+  <si>
+    <t>v2.6</t>
+  </si>
+  <si>
+    <t>v2.7</t>
+  </si>
+  <si>
+    <t>Reviewed DELETEUSER feature</t>
+  </si>
+  <si>
+    <t>LH-SRS-DELETEUSER-006</t>
+  </si>
+  <si>
+    <t>LH-SRS-DELETEUSER-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The message content for a non-matching user is not explicitly defined. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="29">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Roboto"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,110 +676,79 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF404040"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -750,61 +756,36 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,7 +812,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799951170384838"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,198 +824,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799951170384838"/>
-        <bgColor theme="4" tint="0.799951170384838"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
+        <bgColor theme="4" tint="0.79995117038483843"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor theme="4" tint="0.799951170384838"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <bgColor theme="4" tint="0.79995117038483843"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1124,286 +931,47 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1413,16 +981,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="26" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1431,13 +999,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1455,7 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1471,27 +1039,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1512,110 +1080,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="13" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="13" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1873,33 +1470,33 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:K29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="77" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.4285714285714" style="15" customWidth="1"/>
-    <col min="2" max="2" width="19.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="22.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="11.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="85" customWidth="1"/>
-    <col min="7" max="7" width="76.2857142857143" customWidth="1"/>
-    <col min="8" max="8" width="19.1428571428571" customWidth="1"/>
-    <col min="9" max="9" width="21.7142857142857" customWidth="1"/>
-    <col min="10" max="10" width="30.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" ht="18.75" spans="1:10">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="18.75">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1927,11 +1524,11 @@
       <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="53" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="1" ht="60" spans="1:10">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="75">
       <c r="A2" s="18">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1957,14 +1554,14 @@
       <c r="H2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="61" t="s">
+      <c r="I2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" ht="45" spans="1:10">
+      <c r="J2" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45">
       <c r="A3" s="22">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1993,11 +1590,11 @@
       <c r="I3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" ht="30" spans="1:10">
+      <c r="J3" s="57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="18">
         <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
@@ -2023,14 +1620,14 @@
       <c r="H4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" ht="30" spans="1:11">
+      <c r="I4" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2059,12 +1656,12 @@
       <c r="I5" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="64"/>
-    </row>
-    <row r="6" ht="30" spans="1:11">
+      <c r="J5" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="58"/>
+    </row>
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2090,15 +1687,15 @@
       <c r="H6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="64"/>
-    </row>
-    <row r="7" ht="30" spans="1:10">
+      <c r="I6" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="58"/>
+    </row>
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2127,11 +1724,11 @@
       <c r="I7" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" ht="30" spans="1:10">
+      <c r="J7" s="57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2157,14 +1754,14 @@
       <c r="H8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" ht="35.25" customHeight="1" spans="1:10">
+      <c r="I8" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="35.25" customHeight="1">
       <c r="A9" s="30">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2193,11 +1790,11 @@
       <c r="I9" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" ht="45" spans="1:10">
+      <c r="J9" s="57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="18">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -2223,14 +1820,14 @@
       <c r="H10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" ht="30" spans="1:10">
+      <c r="I10" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30">
       <c r="A11" s="30">
         <f>DATE(2025,4,17)</f>
         <v>45764</v>
@@ -2259,11 +1856,11 @@
       <c r="I11" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="63" t="s">
+      <c r="J11" s="57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" ht="45" spans="1:10">
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="36">
         <f t="shared" ref="A12:A14" si="1">DATE(2025,4,17)</f>
         <v>45764</v>
@@ -2289,14 +1886,14 @@
       <c r="H12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" ht="30" spans="1:10">
+      <c r="I12" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="30">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -2325,11 +1922,11 @@
       <c r="I13" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" ht="45" spans="1:10">
+      <c r="J13" s="57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="36">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -2355,14 +1952,14 @@
       <c r="H14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="I14" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="41">
         <v>45765</v>
       </c>
@@ -2387,14 +1984,14 @@
       <c r="H15" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="65" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" ht="30" spans="1:10">
+      <c r="I15" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="36">
         <v>45765</v>
       </c>
@@ -2426,7 +2023,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" ht="30" spans="1:10">
+    <row r="17" spans="1:10" ht="30">
       <c r="A17" s="30">
         <v>45765</v>
       </c>
@@ -2458,7 +2055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="1" spans="1:10">
+    <row r="18" spans="1:10" s="14" customFormat="1">
       <c r="A18" s="51">
         <v>45765</v>
       </c>
@@ -2483,10 +2080,10 @@
       <c r="H18" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="66" t="s">
+      <c r="I18" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="66" t="s">
+      <c r="J18" s="61" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2522,35 +2119,35 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="53">
+    <row r="20" spans="1:10" s="81" customFormat="1">
+      <c r="A20" s="82">
         <v>45785</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="25" t="s">
+      <c r="I20" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="84" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2586,47 +2183,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" ht="75" spans="1:10">
-      <c r="A22" s="54">
+    <row r="22" spans="1:10" s="81" customFormat="1" ht="75">
+      <c r="A22" s="77">
         <v>45786</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="55" t="s">
+      <c r="G22" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="62">
+        <v>45786</v>
+      </c>
+      <c r="B23" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="56" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="54">
-        <v>45786</v>
-      </c>
-      <c r="B23" s="55" t="s">
+      <c r="C23" s="56" t="s">
         <v>103</v>
-      </c>
-      <c r="C23" s="56" t="s">
-        <v>104</v>
       </c>
       <c r="D23" s="56" t="s">
         <v>29</v>
@@ -2635,12 +2232,12 @@
         <v>93</v>
       </c>
       <c r="F23" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="58" t="s">
+      <c r="H23" s="64" t="s">
         <v>16</v>
       </c>
       <c r="I23" s="56" t="s">
@@ -2650,61 +2247,61 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="54">
+    <row r="24" spans="1:10" s="81" customFormat="1">
+      <c r="A24" s="77">
         <v>45786</v>
       </c>
-      <c r="B24" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="58" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="58" t="s">
+      <c r="B24" s="78" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="79" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="H24" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="I24" s="56" t="s">
+      <c r="F24" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" s="79" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="I24" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="56" t="s">
+      <c r="J24" s="79" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="54">
+      <c r="A25" s="62">
         <v>45786</v>
       </c>
-      <c r="B25" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="58" t="s">
+      <c r="B25" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="64" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G25" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="58" t="s">
+      <c r="F25" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="H25" s="64" t="s">
         <v>16</v>
       </c>
       <c r="I25" s="56" t="s">
@@ -2714,62 +2311,62 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="54">
+    <row r="26" spans="1:10" s="81" customFormat="1">
+      <c r="A26" s="77">
         <v>45786</v>
       </c>
-      <c r="B26" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="56" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" t="s">
-        <v>120</v>
-      </c>
-      <c r="G26" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="H26" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="I26" s="56" t="s">
+      <c r="B26" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="G26" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="H26" s="79" t="s">
+        <v>152</v>
+      </c>
+      <c r="I26" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="56" t="s">
+      <c r="J26" s="79" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" ht="45" spans="1:10">
-      <c r="A27" s="54">
+    <row r="27" spans="1:10" ht="45">
+      <c r="A27" s="62">
         <v>45786</v>
       </c>
-      <c r="B27" s="55" t="s">
-        <v>123</v>
+      <c r="B27" s="59" t="s">
+        <v>154</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="D27" s="56" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E27" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="57" t="s">
-        <v>126</v>
+        <v>146</v>
+      </c>
+      <c r="F27" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="G27" s="63" t="s">
+        <v>156</v>
       </c>
       <c r="H27" s="56" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="I27" s="56" t="s">
         <v>58</v>
@@ -2778,31 +2375,200 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="55"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="55"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
+    <row r="28" spans="1:10" s="70" customFormat="1" ht="60">
+      <c r="A28" s="66">
+        <v>45786</v>
+      </c>
+      <c r="B28" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="H28" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="I28" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="76" customFormat="1" ht="60">
+      <c r="A29" s="71">
+        <v>45786</v>
+      </c>
+      <c r="B29" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="H29" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="I29" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J29" s="75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="81" customFormat="1" ht="60">
+      <c r="A30" s="77">
+        <v>45786</v>
+      </c>
+      <c r="B30" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="79" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="91" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="G30" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="79" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="76" customFormat="1" ht="90">
+      <c r="A31" s="71">
+        <v>45786</v>
+      </c>
+      <c r="B31" s="72" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="92" t="s">
+        <v>182</v>
+      </c>
+      <c r="F31" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="G31" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="81" customFormat="1" ht="60">
+      <c r="A32" s="77">
+        <v>45786</v>
+      </c>
+      <c r="B32" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="91" t="s">
+        <v>182</v>
+      </c>
+      <c r="F32" s="80" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="79" t="s">
+        <v>179</v>
+      </c>
+      <c r="H32" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="J32" s="79" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="81" customFormat="1" ht="30">
+      <c r="A33" s="77">
+        <v>45787</v>
+      </c>
+      <c r="B33" s="89" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="91" t="s">
+        <v>185</v>
+      </c>
+      <c r="D33" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="91" t="s">
+        <v>182</v>
+      </c>
+      <c r="F33" s="90" t="s">
+        <v>186</v>
+      </c>
+      <c r="G33" s="88" t="s">
+        <v>186</v>
+      </c>
+      <c r="H33" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="J33" s="79" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15">
       <formula1>"open,in progress,closed,not applicable"</formula1>
@@ -2812,56 +2578,54 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="33.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="78.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="23.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" spans="1:4">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" ht="18.75" spans="1:4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
       </c>
     </row>
-    <row r="3" ht="75" spans="1:4">
+    <row r="3" spans="1:4" ht="75">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -2869,167 +2633,167 @@
         <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D3" s="8">
         <v>45761</v>
       </c>
     </row>
-    <row r="4" ht="18.75" spans="1:4">
+    <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="9" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D4" s="11">
         <v>45761</v>
       </c>
     </row>
-    <row r="5" ht="18.75" spans="1:4">
+    <row r="5" spans="1:4" ht="18.75">
       <c r="A5" s="9" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="D5" s="11">
         <v>45764</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="1:4">
+    <row r="6" spans="1:4" ht="18.75">
       <c r="A6" s="9" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="D6" s="11">
         <v>45765</v>
       </c>
     </row>
-    <row r="7" ht="18.75" spans="1:4">
+    <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="D7" s="5">
         <v>45765</v>
       </c>
     </row>
-    <row r="8" ht="18.75" spans="1:4">
+    <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="3" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="D8" s="5">
         <v>45765</v>
       </c>
     </row>
-    <row r="9" ht="37.5" spans="1:4">
+    <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="D9" s="5">
         <v>45766</v>
       </c>
     </row>
-    <row r="10" ht="18.75" spans="1:4">
+    <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="D10" s="5">
         <v>45766</v>
       </c>
     </row>
-    <row r="11" ht="18.75" spans="1:4">
+    <row r="11" spans="1:4" ht="18.75">
       <c r="A11" s="3" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="D11" s="5">
         <v>45767</v>
       </c>
     </row>
-    <row r="12" ht="18.75" spans="1:4">
+    <row r="12" spans="1:4" ht="18.75">
       <c r="A12" s="3" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="D12" s="5">
         <v>45785</v>
       </c>
     </row>
-    <row r="13" ht="18.75" spans="1:4">
+    <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D13" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="14" ht="18.75" spans="1:4">
+    <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D14" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="15" ht="18.75" spans="1:4">
+    <row r="15" spans="1:4" ht="18.75">
       <c r="A15" s="3" t="s">
         <v>93</v>
       </c>
@@ -3037,15 +2801,15 @@
         <v>72</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D15" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="16" ht="18.75" spans="1:4">
+    <row r="16" spans="1:4" ht="18.75">
       <c r="A16" s="3" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>157</v>
@@ -3057,22 +2821,50 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="17" ht="18.75" spans="1:4">
+    <row r="17" spans="1:4" ht="18.75">
       <c r="A17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="D17" s="5">
         <v>45786</v>
       </c>
     </row>
+    <row r="18" spans="1:4" ht="18.75">
+      <c r="A18" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="86" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="87">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75">
+      <c r="A19" s="85" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="86" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="87">
+        <v>45786</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v2.9 closed owner reviews
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6FB01F-8A7F-4B0A-AEBF-268770883167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -19,8 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="190">
   <si>
     <t>date</t>
   </si>
@@ -664,18 +668,15 @@
   <si>
     <t>Closed owner review</t>
   </si>
+  <si>
+    <t>v2.9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="29">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,150 +734,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -891,8 +748,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -919,7 +789,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799951170384838"/>
+        <fgColor theme="4" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,198 +801,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799951170384838"/>
-        <bgColor theme="4" tint="0.799951170384838"/>
+        <fgColor theme="4" tint="0.79992065187536243"/>
+        <bgColor theme="4" tint="0.79992065187536243"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor theme="4" tint="0.799951170384838"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <bgColor theme="4" tint="0.79992065187536243"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1212,251 +902,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1498,9 +949,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="26"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="26" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="26" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1510,10 +960,10 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="26" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1522,7 +972,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1546,7 +996,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1562,7 +1012,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1573,7 +1023,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1603,34 +1053,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="0" xfId="26" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="26" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="26" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="5" borderId="1" xfId="26" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="26" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="26" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="26" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1639,46 +1089,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="5" fillId="5" borderId="1" xfId="26" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="4" borderId="1" xfId="26" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1702,65 +1122,48 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="26" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2018,1135 +1421,1133 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="81" topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView topLeftCell="A20" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.4285714285714" style="18" customWidth="1"/>
-    <col min="2" max="2" width="24.6857142857143" customWidth="1"/>
-    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="22.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="11.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="85" customWidth="1"/>
-    <col min="7" max="7" width="76.2857142857143" customWidth="1"/>
-    <col min="8" max="8" width="19.1428571428571" customWidth="1"/>
-    <col min="9" max="9" width="21.7142857142857" customWidth="1"/>
-    <col min="10" max="10" width="30.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="76.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" ht="18.75" spans="1:10">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="18">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="80" t="s">
+      <c r="J1" s="69" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="1" ht="60" spans="1:10">
-      <c r="A2" s="21">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="57.6">
+      <c r="A2" s="20">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="82" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" ht="45" spans="1:10">
-      <c r="A3" s="25">
+      <c r="J2" s="71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.2">
+      <c r="A3" s="24">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" ht="30" spans="1:10">
-      <c r="A4" s="21">
+      <c r="I3" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8">
+      <c r="A4" s="20">
         <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="82" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" ht="30" spans="1:11">
-      <c r="A5" s="33">
+      <c r="I4" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8">
+      <c r="A5" s="32">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="84"/>
-    </row>
-    <row r="6" ht="30" spans="1:11">
-      <c r="A6" s="21">
+      <c r="I5" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="73"/>
+    </row>
+    <row r="6" spans="1:11" ht="28.8">
+      <c r="A6" s="20">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="82" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="84"/>
-    </row>
-    <row r="7" ht="30" spans="1:10">
-      <c r="A7" s="33">
+      <c r="I6" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="73"/>
+    </row>
+    <row r="7" spans="1:11" ht="28.8">
+      <c r="A7" s="32">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" ht="30" spans="1:10">
-      <c r="A8" s="21">
+      <c r="I7" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.8">
+      <c r="A8" s="20">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="82" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" ht="35.25" customHeight="1" spans="1:10">
-      <c r="A9" s="33">
+      <c r="I8" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="35.25" customHeight="1">
+      <c r="A9" s="32">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" ht="45" spans="1:10">
-      <c r="A10" s="21">
+      <c r="I9" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.8">
+      <c r="A10" s="20">
         <f t="shared" si="0"/>
         <v>45761</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="82" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" ht="30" spans="1:10">
-      <c r="A11" s="33">
+      <c r="I10" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28.8">
+      <c r="A11" s="32">
         <f>DATE(2025,4,17)</f>
         <v>45764</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="83" t="s">
+      <c r="I11" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="72" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" ht="45" spans="1:10">
-      <c r="A12" s="39">
+    <row r="12" spans="1:11" ht="43.2">
+      <c r="A12" s="38">
         <f t="shared" ref="A12:A14" si="1">DATE(2025,4,17)</f>
         <v>45764</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="82" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" ht="30" spans="1:10">
-      <c r="A13" s="33">
+      <c r="I12" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8">
+      <c r="A13" s="32">
         <f t="shared" si="1"/>
         <v>45764</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="H13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" ht="45" spans="1:10">
-      <c r="A14" s="39">
+      <c r="I13" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="43.2">
+      <c r="A14" s="38">
         <f t="shared" si="1"/>
         <v>45764</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="82" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="44">
+      <c r="I14" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="43">
         <v>45765</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="48" t="s">
+      <c r="G15" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="46" t="s">
+      <c r="H15" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="85" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" ht="30" spans="1:10">
-      <c r="A16" s="39">
+      <c r="I15" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="74" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8">
+      <c r="A16" s="38">
         <v>45765</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="50" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" ht="30" spans="1:10">
-      <c r="A17" s="33">
+      <c r="I16" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28.8">
+      <c r="A17" s="32">
         <v>45765</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="53" t="s">
+      <c r="G17" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="46" t="s">
+      <c r="H17" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="46" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" s="14" customFormat="1" spans="1:10">
-      <c r="A18" s="54">
+      <c r="I17" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="14" customFormat="1">
+      <c r="A18" s="53">
         <v>45765</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="55" t="s">
+      <c r="G18" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="50" t="s">
+      <c r="H18" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="86" t="s">
+      <c r="I18" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="86" t="s">
+      <c r="J18" s="75" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33">
+      <c r="A19" s="32">
         <v>45765</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="46" t="s">
+      <c r="H19" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="J19" s="27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" s="15" customFormat="1" spans="1:10">
-      <c r="A20" s="56">
+    <row r="20" spans="1:10" s="15" customFormat="1">
+      <c r="A20" s="55">
         <v>45785</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F20" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="58" t="s">
+      <c r="H20" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="58" t="s">
+      <c r="I20" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="57" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="33">
+      <c r="A21" s="32">
         <v>45786</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="H21" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" s="15" customFormat="1" ht="75" spans="1:10">
-      <c r="A22" s="59">
+      <c r="I21" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="15" customFormat="1" ht="72">
+      <c r="A22" s="58">
         <v>45786</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="62" t="s">
+      <c r="F22" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="60" t="s">
+      <c r="G22" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="61" t="s">
+      <c r="H22" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="77" t="s">
+      <c r="I22" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="60" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="63">
+      <c r="A23" s="62">
         <v>45786</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="65" t="s">
+      <c r="F23" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="65" t="s">
+      <c r="G23" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="H23" s="66" t="s">
+      <c r="H23" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="65" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" s="15" customFormat="1" spans="1:10">
-      <c r="A24" s="59">
+      <c r="I23" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="15" customFormat="1">
+      <c r="A24" s="58">
         <v>45786</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="61" t="s">
+      <c r="F24" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="G24" s="61" t="s">
+      <c r="G24" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="H24" s="61" t="s">
+      <c r="H24" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="I24" s="61" t="s">
+      <c r="I24" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="61" t="s">
+      <c r="J24" s="60" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="63">
+      <c r="A25" s="62">
         <v>45786</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="66" t="s">
+      <c r="D25" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="66" t="s">
+      <c r="F25" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="G25" s="66" t="s">
+      <c r="G25" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="66" t="s">
+      <c r="H25" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="65" t="s">
+      <c r="I25" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="65" t="s">
+      <c r="J25" s="64" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" s="15" customFormat="1" spans="1:10">
-      <c r="A26" s="59">
+    <row r="26" spans="1:10" s="16" customFormat="1">
+      <c r="A26" s="65">
         <v>45786</v>
       </c>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="61" t="s">
+      <c r="D26" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="61" t="s">
+      <c r="E26" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="G26" s="61" t="s">
+      <c r="G26" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="H26" s="61" t="s">
+      <c r="H26" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="I26" s="61" t="s">
+      <c r="I26" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="86" customFormat="1" ht="28.8">
+      <c r="A27" s="81">
+        <v>45786</v>
+      </c>
+      <c r="B27" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="83" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="80" customFormat="1" ht="57.6">
+      <c r="A28" s="76">
+        <v>45786</v>
+      </c>
+      <c r="B28" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="79" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" s="78" t="s">
+        <v>130</v>
+      </c>
+      <c r="I28" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="78" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="16" customFormat="1" ht="57.6">
+      <c r="A29" s="65">
+        <v>45786</v>
+      </c>
+      <c r="B29" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="I29" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="15" customFormat="1" ht="57.6">
+      <c r="A30" s="58">
+        <v>45786</v>
+      </c>
+      <c r="B30" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="H30" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="61" t="s">
+    </row>
+    <row r="31" spans="1:10" s="16" customFormat="1" ht="86.4">
+      <c r="A31" s="65">
+        <v>45786</v>
+      </c>
+      <c r="B31" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="67" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" ht="45" spans="1:10">
-      <c r="A27" s="63">
+    <row r="32" spans="1:10" s="15" customFormat="1" ht="57.6">
+      <c r="A32" s="58">
         <v>45786</v>
       </c>
-      <c r="B27" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" s="65" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="H27" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="I27" s="65" t="s">
+      <c r="B32" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="H32" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="J27" s="65" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" s="16" customFormat="1" ht="60" spans="1:10">
-      <c r="A28" s="69">
-        <v>45786</v>
-      </c>
-      <c r="B28" s="70" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="71" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" s="71" t="s">
+    </row>
+    <row r="33" spans="1:10" s="15" customFormat="1">
+      <c r="A33" s="58">
+        <v>45787</v>
+      </c>
+      <c r="B33" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="71" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="I28" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="J28" s="71" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" s="17" customFormat="1" ht="60" spans="1:10">
-      <c r="A29" s="73">
-        <v>45786</v>
-      </c>
-      <c r="B29" s="74" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="75" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="G29" s="75" t="s">
-        <v>133</v>
-      </c>
-      <c r="H29" s="75" t="s">
-        <v>130</v>
-      </c>
-      <c r="I29" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="J29" s="87" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" s="15" customFormat="1" ht="60" spans="1:10">
-      <c r="A30" s="59">
-        <v>45786</v>
-      </c>
-      <c r="B30" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="61" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="77" t="s">
+      <c r="E33" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="62" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="61" t="s">
-        <v>138</v>
-      </c>
-      <c r="H30" s="61" t="s">
+      <c r="F33" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="H33" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I30" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="61" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" s="17" customFormat="1" ht="90" spans="1:10">
-      <c r="A31" s="73">
-        <v>45786</v>
-      </c>
-      <c r="B31" s="74" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="D31" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="75" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="76" t="s">
-        <v>141</v>
-      </c>
-      <c r="G31" s="75" t="s">
-        <v>142</v>
-      </c>
-      <c r="H31" s="75" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="87" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="87" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" s="15" customFormat="1" ht="60" spans="1:10">
-      <c r="A32" s="59">
-        <v>45786</v>
-      </c>
-      <c r="B32" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="61" t="s">
-        <v>144</v>
-      </c>
-      <c r="D32" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="F32" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="G32" s="61" t="s">
-        <v>146</v>
-      </c>
-      <c r="H32" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="I32" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="61" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" s="15" customFormat="1" spans="1:10">
-      <c r="A33" s="59">
-        <v>45787</v>
-      </c>
-      <c r="B33" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="78" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" s="79" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="77" t="s">
-        <v>149</v>
-      </c>
-      <c r="H33" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="I33" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="61" t="s">
+      <c r="I33" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="60" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="33.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="78.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="23.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" spans="1:4">
+    <row r="1" spans="1:4" ht="21">
       <c r="A1" s="1" t="s">
         <v>150</v>
       </c>
@@ -3160,7 +2561,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:4">
+    <row r="2" spans="1:4" ht="18.600000000000001">
       <c r="A2" s="3" t="s">
         <v>154</v>
       </c>
@@ -3174,7 +2575,7 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="3" ht="75" spans="1:4">
+    <row r="3" spans="1:4" ht="74.400000000000006">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -3188,7 +2589,7 @@
         <v>45761</v>
       </c>
     </row>
-    <row r="4" ht="18.75" spans="1:4">
+    <row r="4" spans="1:4" ht="18.600000000000001">
       <c r="A4" s="9" t="s">
         <v>157</v>
       </c>
@@ -3202,7 +2603,7 @@
         <v>45761</v>
       </c>
     </row>
-    <row r="5" ht="18.75" spans="1:4">
+    <row r="5" spans="1:4" ht="18.600000000000001">
       <c r="A5" s="9" t="s">
         <v>159</v>
       </c>
@@ -3216,7 +2617,7 @@
         <v>45764</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="1:4">
+    <row r="6" spans="1:4" ht="18.600000000000001">
       <c r="A6" s="9" t="s">
         <v>161</v>
       </c>
@@ -3230,7 +2631,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="7" ht="18.75" spans="1:4">
+    <row r="7" spans="1:4" ht="18.600000000000001">
       <c r="A7" s="3" t="s">
         <v>163</v>
       </c>
@@ -3244,7 +2645,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="8" ht="18.75" spans="1:4">
+    <row r="8" spans="1:4" ht="18.600000000000001">
       <c r="A8" s="3" t="s">
         <v>165</v>
       </c>
@@ -3258,7 +2659,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="9" ht="37.5" spans="1:4">
+    <row r="9" spans="1:4" ht="37.200000000000003">
       <c r="A9" s="3" t="s">
         <v>167</v>
       </c>
@@ -3272,7 +2673,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="10" ht="18.75" spans="1:4">
+    <row r="10" spans="1:4" ht="18.600000000000001">
       <c r="A10" s="3" t="s">
         <v>169</v>
       </c>
@@ -3286,7 +2687,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="11" ht="18.75" spans="1:4">
+    <row r="11" spans="1:4" ht="18.600000000000001">
       <c r="A11" s="3" t="s">
         <v>171</v>
       </c>
@@ -3300,7 +2701,7 @@
         <v>45767</v>
       </c>
     </row>
-    <row r="12" ht="18.75" spans="1:4">
+    <row r="12" spans="1:4" ht="18.600000000000001">
       <c r="A12" s="3" t="s">
         <v>173</v>
       </c>
@@ -3314,7 +2715,7 @@
         <v>45785</v>
       </c>
     </row>
-    <row r="13" ht="18.75" spans="1:4">
+    <row r="13" spans="1:4" ht="18.600000000000001">
       <c r="A13" s="3" t="s">
         <v>175</v>
       </c>
@@ -3328,7 +2729,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="14" ht="18.75" spans="1:4">
+    <row r="14" spans="1:4" ht="18.600000000000001">
       <c r="A14" s="3" t="s">
         <v>177</v>
       </c>
@@ -3342,7 +2743,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="15" ht="18.75" spans="1:4">
+    <row r="15" spans="1:4" ht="18.600000000000001">
       <c r="A15" s="3" t="s">
         <v>93</v>
       </c>
@@ -3356,7 +2757,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="16" ht="18.75" spans="1:4">
+    <row r="16" spans="1:4" ht="18.600000000000001">
       <c r="A16" s="3" t="s">
         <v>119</v>
       </c>
@@ -3370,7 +2771,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="17" ht="18.75" spans="1:4">
+    <row r="17" spans="1:4" ht="18.600000000000001">
       <c r="A17" s="3" t="s">
         <v>182</v>
       </c>
@@ -3384,7 +2785,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="18" ht="18.75" spans="1:4">
+    <row r="18" spans="1:4" ht="18.600000000000001">
       <c r="A18" s="3" t="s">
         <v>184</v>
       </c>
@@ -3398,7 +2799,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="19" ht="18.75" spans="1:4">
+    <row r="19" spans="1:4" ht="18.600000000000001">
       <c r="A19" s="3" t="s">
         <v>136</v>
       </c>
@@ -3412,7 +2813,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="20" ht="18.75" spans="1:4">
+    <row r="20" spans="1:4" ht="18.600000000000001">
       <c r="A20" s="3" t="s">
         <v>187</v>
       </c>
@@ -3426,8 +2827,22 @@
         <v>45787</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="18.600000000000001">
+      <c r="A21" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="5">
+        <v>45787</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v3.0 Closed reviewer verification for Login , Delete user and CATEGORIES features
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6FB01F-8A7F-4B0A-AEBF-268770883167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="192">
   <si>
     <t>date</t>
   </si>
@@ -671,11 +670,17 @@
   <si>
     <t>v2.9</t>
   </si>
+  <si>
+    <t>v3.0</t>
+  </si>
+  <si>
+    <t>Closed reviewer verification for Login , Delete user and CATEGORIES features</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -907,7 +912,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1151,6 +1156,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1426,28 +1437,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A25" zoomScale="45" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="85" customWidth="1"/>
-    <col min="7" max="7" width="76.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="10" max="10" width="30.88671875" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="18">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="18.75">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1479,7 +1490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="13" customFormat="1" ht="57.6">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="75">
       <c r="A2" s="20">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1512,7 +1523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.2">
+    <row r="3" spans="1:11" ht="45">
       <c r="A3" s="24">
         <f>DATE(2025,4,13)</f>
         <v>45760</v>
@@ -1545,7 +1556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="20">
         <f t="shared" ref="A4:A10" si="0">DATE(2025,4,14)</f>
         <v>45761</v>
@@ -1578,7 +1589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8">
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="32">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1612,7 +1623,7 @@
       </c>
       <c r="K5" s="73"/>
     </row>
-    <row r="6" spans="1:11" ht="28.8">
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="20">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1646,7 +1657,7 @@
       </c>
       <c r="K6" s="73"/>
     </row>
-    <row r="7" spans="1:11" ht="28.8">
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="32">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1679,7 +1690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8">
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="20">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1745,7 +1756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8">
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="20">
         <f t="shared" si="0"/>
         <v>45761</v>
@@ -1778,7 +1789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8">
+    <row r="11" spans="1:11" ht="30">
       <c r="A11" s="32">
         <f>DATE(2025,4,17)</f>
         <v>45764</v>
@@ -1811,7 +1822,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43.2">
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="38">
         <f t="shared" ref="A12:A14" si="1">DATE(2025,4,17)</f>
         <v>45764</v>
@@ -1844,7 +1855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8">
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="32">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -1877,7 +1888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="43.2">
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="38">
         <f t="shared" si="1"/>
         <v>45764</v>
@@ -1942,7 +1953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="38">
         <v>45765</v>
       </c>
@@ -1974,7 +1985,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="28.8">
+    <row r="17" spans="1:10" ht="30">
       <c r="A17" s="32">
         <v>45765</v>
       </c>
@@ -2134,7 +2145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="15" customFormat="1" ht="72">
+    <row r="22" spans="1:10" s="15" customFormat="1" ht="75">
       <c r="A22" s="58">
         <v>45786</v>
       </c>
@@ -2294,7 +2305,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="86" customFormat="1" ht="28.8">
+    <row r="27" spans="1:10" s="86" customFormat="1" ht="45">
       <c r="A27" s="81">
         <v>45786</v>
       </c>
@@ -2326,7 +2337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="80" customFormat="1" ht="57.6">
+    <row r="28" spans="1:10" s="80" customFormat="1" ht="60">
       <c r="A28" s="76">
         <v>45786</v>
       </c>
@@ -2358,7 +2369,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="16" customFormat="1" ht="57.6">
+    <row r="29" spans="1:10" s="16" customFormat="1" ht="60">
       <c r="A29" s="65">
         <v>45786</v>
       </c>
@@ -2390,7 +2401,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="15" customFormat="1" ht="57.6">
+    <row r="30" spans="1:10" s="15" customFormat="1" ht="60">
       <c r="A30" s="58">
         <v>45786</v>
       </c>
@@ -2418,11 +2429,11 @@
       <c r="I30" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="16" customFormat="1" ht="86.4">
+      <c r="J30" s="87" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="16" customFormat="1" ht="90">
       <c r="A31" s="65">
         <v>45786</v>
       </c>
@@ -2450,11 +2461,11 @@
       <c r="I31" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="J31" s="67" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="15" customFormat="1" ht="57.6">
+      <c r="J31" s="88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="15" customFormat="1" ht="60">
       <c r="A32" s="58">
         <v>45786</v>
       </c>
@@ -2482,8 +2493,8 @@
       <c r="I32" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="60" t="s">
-        <v>58</v>
+      <c r="J32" s="87" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="15" customFormat="1">
@@ -2514,16 +2525,16 @@
       <c r="I33" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="60" t="s">
-        <v>58</v>
+      <c r="J33" s="87" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I15">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J15">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2532,22 +2543,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B27" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="78.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>150</v>
       </c>
@@ -2561,7 +2572,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.600000000000001">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>154</v>
       </c>
@@ -2575,7 +2586,7 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="74.400000000000006">
+    <row r="3" spans="1:4" ht="75">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -2589,7 +2600,7 @@
         <v>45761</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001">
+    <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="9" t="s">
         <v>157</v>
       </c>
@@ -2603,7 +2614,7 @@
         <v>45761</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.600000000000001">
+    <row r="5" spans="1:4" ht="18.75">
       <c r="A5" s="9" t="s">
         <v>159</v>
       </c>
@@ -2617,7 +2628,7 @@
         <v>45764</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.600000000000001">
+    <row r="6" spans="1:4" ht="18.75">
       <c r="A6" s="9" t="s">
         <v>161</v>
       </c>
@@ -2631,7 +2642,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.600000000000001">
+    <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="3" t="s">
         <v>163</v>
       </c>
@@ -2645,7 +2656,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.600000000000001">
+    <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>165</v>
       </c>
@@ -2659,7 +2670,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.200000000000003">
+    <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
         <v>167</v>
       </c>
@@ -2673,7 +2684,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.600000000000001">
+    <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="3" t="s">
         <v>169</v>
       </c>
@@ -2687,7 +2698,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.600000000000001">
+    <row r="11" spans="1:4" ht="18.75">
       <c r="A11" s="3" t="s">
         <v>171</v>
       </c>
@@ -2701,7 +2712,7 @@
         <v>45767</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.600000000000001">
+    <row r="12" spans="1:4" ht="18.75">
       <c r="A12" s="3" t="s">
         <v>173</v>
       </c>
@@ -2715,7 +2726,7 @@
         <v>45785</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.600000000000001">
+    <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="3" t="s">
         <v>175</v>
       </c>
@@ -2729,7 +2740,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.600000000000001">
+    <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>177</v>
       </c>
@@ -2743,7 +2754,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18.600000000000001">
+    <row r="15" spans="1:4" ht="18.75">
       <c r="A15" s="3" t="s">
         <v>93</v>
       </c>
@@ -2757,7 +2768,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18.600000000000001">
+    <row r="16" spans="1:4" ht="18.75">
       <c r="A16" s="3" t="s">
         <v>119</v>
       </c>
@@ -2771,7 +2782,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18.600000000000001">
+    <row r="17" spans="1:4" ht="18.75">
       <c r="A17" s="3" t="s">
         <v>182</v>
       </c>
@@ -2785,7 +2796,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18.600000000000001">
+    <row r="18" spans="1:4" ht="18.75">
       <c r="A18" s="3" t="s">
         <v>184</v>
       </c>
@@ -2799,7 +2810,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18.600000000000001">
+    <row r="19" spans="1:4" ht="18.75">
       <c r="A19" s="3" t="s">
         <v>136</v>
       </c>
@@ -2813,7 +2824,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18.600000000000001">
+    <row r="20" spans="1:4" ht="18.75">
       <c r="A20" s="3" t="s">
         <v>187</v>
       </c>
@@ -2827,7 +2838,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18.600000000000001">
+    <row r="21" spans="1:4" ht="18.75">
       <c r="A21" s="3" t="s">
         <v>189</v>
       </c>
@@ -2838,6 +2849,20 @@
         <v>188</v>
       </c>
       <c r="D21" s="5">
+        <v>45787</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="37.5">
+      <c r="A22" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="5">
         <v>45787</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v3.1 Reviewed SYSTEMCONSTRAINS and NOTIFICATION SRS Features  ,,  no comments
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="194">
   <si>
     <t>date</t>
   </si>
@@ -675,6 +675,12 @@
   </si>
   <si>
     <t>Closed reviewer verification for Login , Delete user and CATEGORIES features</t>
+  </si>
+  <si>
+    <t>v3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed SYSTEMCONSTRAINS and NOTIFICATION SRS Features  ,,  no comments </t>
   </si>
 </sst>
 </file>
@@ -1440,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="45" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView topLeftCell="A28" zoomScale="61" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2544,10 +2550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B27" sqref="A1:XFD1048576"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2866,6 +2872,20 @@
         <v>45787</v>
       </c>
     </row>
+    <row r="23" spans="1:4" ht="37.5">
+      <c r="A23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="5">
+        <v>45787</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v3.2 Reviewed USERHOME  and ADMINHOME SRS Features, NO comments
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_SRS_REVIEWS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="191">
   <si>
     <t>date</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Recommendation: The message should be shown in a bigger area like next to the password field or in a popup</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>LH-REVIEW-SRS-011</t>
@@ -432,18 +429,6 @@
     <t>Mahmoud</t>
   </si>
   <si>
-    <t>LH-REVIEW-SRS-024</t>
-  </si>
-  <si>
-    <t>SRS-ADMIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naming like LH-SRS-DELETEPOST what is deletpost </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use namig by the name of the feature ADMIN Constrains </t>
-  </si>
-  <si>
     <t>LH-REVIEW-SRS-025</t>
   </si>
   <si>
@@ -638,9 +623,6 @@
     <t>Reviewed publish Audio</t>
   </si>
   <si>
-    <t xml:space="preserve">Reviewed publish Video &amp; Admin Home </t>
-  </si>
-  <si>
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
@@ -680,7 +662,16 @@
     <t>v3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Reviewed SYSTEMCONSTRAINS and NOTIFICATION SRS Features  ,,  no comments </t>
+    <t>v3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed SYSTEMCONSTRAINS and NOTIFICATION SRS Features ,No comments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed USERHOME  and ADMINHOME SRS Features, NO comments </t>
+  </si>
+  <si>
+    <t>Reviewed publish Video</t>
   </si>
 </sst>
 </file>
@@ -918,7 +909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1167,6 +1158,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1444,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="61" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A23" zoomScale="50" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1825,7 +1819,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="72" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45">
@@ -1834,10 +1828,10 @@
         <v>45764</v>
       </c>
       <c r="B12" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>59</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>60</v>
       </c>
       <c r="D12" s="39" t="s">
         <v>55</v>
@@ -1846,10 +1840,10 @@
         <v>30</v>
       </c>
       <c r="F12" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="35" t="s">
         <v>61</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>62</v>
       </c>
       <c r="H12" s="22" t="s">
         <v>16</v>
@@ -1867,10 +1861,10 @@
         <v>45764</v>
       </c>
       <c r="B13" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>63</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>64</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>55</v>
@@ -1879,10 +1873,10 @@
         <v>30</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="27" t="s">
         <v>16</v>
@@ -1900,10 +1894,10 @@
         <v>45764</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D14" s="39" t="s">
         <v>55</v>
@@ -1912,10 +1906,10 @@
         <v>30</v>
       </c>
       <c r="F14" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="35" t="s">
         <v>68</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>69</v>
       </c>
       <c r="H14" s="22" t="s">
         <v>16</v>
@@ -1932,22 +1926,22 @@
         <v>45765</v>
       </c>
       <c r="B15" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="D15" s="45" t="s">
         <v>71</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>72</v>
       </c>
       <c r="E15" s="45" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="47" t="s">
         <v>73</v>
-      </c>
-      <c r="G15" s="47" t="s">
-        <v>74</v>
       </c>
       <c r="H15" s="45" t="s">
         <v>16</v>
@@ -1964,22 +1958,22 @@
         <v>45765</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="49" t="s">
         <v>71</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>72</v>
       </c>
       <c r="E16" s="49" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="51" t="s">
         <v>76</v>
-      </c>
-      <c r="G16" s="51" t="s">
-        <v>77</v>
       </c>
       <c r="H16" s="49" t="s">
         <v>16</v>
@@ -1996,22 +1990,22 @@
         <v>45765</v>
       </c>
       <c r="B17" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="44" t="s">
-        <v>79</v>
-      </c>
       <c r="D17" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="52" t="s">
         <v>80</v>
-      </c>
-      <c r="G17" s="52" t="s">
-        <v>81</v>
       </c>
       <c r="H17" s="45" t="s">
         <v>16</v>
@@ -2028,31 +2022,31 @@
         <v>45765</v>
       </c>
       <c r="B18" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="D18" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="49" t="s">
+      <c r="F18" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="G18" s="54" t="s">
         <v>85</v>
-      </c>
-      <c r="G18" s="54" t="s">
-        <v>86</v>
       </c>
       <c r="H18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="75" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="J18" s="75" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2060,31 +2054,31 @@
         <v>45765</v>
       </c>
       <c r="B19" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="D19" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="36" t="s">
+      <c r="G19" s="36" t="s">
         <v>89</v>
-      </c>
-      <c r="G19" s="36" t="s">
-        <v>90</v>
       </c>
       <c r="H19" s="45" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="15" customFormat="1">
@@ -2092,25 +2086,25 @@
         <v>45785</v>
       </c>
       <c r="B20" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="56" t="s">
         <v>91</v>
-      </c>
-      <c r="C20" s="56" t="s">
-        <v>92</v>
       </c>
       <c r="D20" s="57" t="s">
         <v>55</v>
       </c>
       <c r="E20" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="G20" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="57" t="s">
+      <c r="H20" s="57" t="s">
         <v>95</v>
-      </c>
-      <c r="H20" s="57" t="s">
-        <v>96</v>
       </c>
       <c r="I20" s="57" t="s">
         <v>18</v>
@@ -2124,22 +2118,22 @@
         <v>45786</v>
       </c>
       <c r="B21" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>98</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="G21" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>95</v>
       </c>
       <c r="H21" s="27" t="s">
         <v>16</v>
@@ -2156,22 +2150,22 @@
         <v>45786</v>
       </c>
       <c r="B22" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="60" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>100</v>
       </c>
       <c r="D22" s="60" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F22" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="59" t="s">
         <v>101</v>
-      </c>
-      <c r="G22" s="59" t="s">
-        <v>102</v>
       </c>
       <c r="H22" s="60" t="s">
         <v>16</v>
@@ -2188,22 +2182,22 @@
         <v>45786</v>
       </c>
       <c r="B23" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="64" t="s">
         <v>103</v>
-      </c>
-      <c r="C23" s="64" t="s">
-        <v>104</v>
       </c>
       <c r="D23" s="64" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F23" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="64" t="s">
         <v>105</v>
-      </c>
-      <c r="G23" s="64" t="s">
-        <v>106</v>
       </c>
       <c r="H23" s="64" t="s">
         <v>16</v>
@@ -2220,318 +2214,286 @@
         <v>45786</v>
       </c>
       <c r="B24" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="D24" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="60" t="s">
+      <c r="G24" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="G24" s="60" t="s">
+      <c r="H24" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="H24" s="60" t="s">
+      <c r="I24" s="87" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="87" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="16" customFormat="1">
+      <c r="A25" s="65">
+        <v>45786</v>
+      </c>
+      <c r="B25" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="I24" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="J24" s="60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="62">
+      <c r="C25" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G25" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="I25" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="86" customFormat="1" ht="45">
+      <c r="A26" s="81">
         <v>45786</v>
       </c>
-      <c r="B25" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="64" t="s">
+      <c r="B26" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="64" t="s">
+      <c r="E26" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="G25" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="J25" s="64" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="16" customFormat="1">
-      <c r="A26" s="65">
+      <c r="F26" s="84" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="85" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I26" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="83" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="80" customFormat="1" ht="60">
+      <c r="A27" s="76">
         <v>45786</v>
       </c>
-      <c r="B26" s="66" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="67" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" s="67" t="s">
+      <c r="B27" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="78" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="16" customFormat="1" ht="60">
+      <c r="A28" s="65">
+        <v>45786</v>
+      </c>
+      <c r="B28" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="67" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="G26" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="H26" s="67" t="s">
-        <v>122</v>
-      </c>
-      <c r="I26" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="67" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="86" customFormat="1" ht="45">
-      <c r="A27" s="81">
+      <c r="C28" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="89" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="15" customFormat="1" ht="60">
+      <c r="A29" s="58">
         <v>45786</v>
       </c>
-      <c r="B27" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" s="83" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" s="83" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" s="84" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="85" t="s">
-        <v>126</v>
-      </c>
-      <c r="H27" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="I27" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="80" customFormat="1" ht="60">
-      <c r="A28" s="76">
+      <c r="B29" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="60" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="87" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="16" customFormat="1" ht="90">
+      <c r="A30" s="65">
         <v>45786</v>
       </c>
-      <c r="B28" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" s="78" t="s">
+      <c r="B30" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="79" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="78" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="78" t="s">
-        <v>130</v>
-      </c>
-      <c r="I28" s="78" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="78" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="16" customFormat="1" ht="60">
-      <c r="A29" s="65">
+      <c r="E30" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="15" customFormat="1" ht="60">
+      <c r="A31" s="58">
         <v>45786</v>
       </c>
-      <c r="B29" s="66" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="67" t="s">
+      <c r="B31" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="67" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" s="68" t="s">
-        <v>132</v>
-      </c>
-      <c r="G29" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="H29" s="67" t="s">
-        <v>130</v>
-      </c>
-      <c r="I29" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="J29" s="67" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="15" customFormat="1" ht="60">
-      <c r="A30" s="58">
-        <v>45786</v>
-      </c>
-      <c r="B30" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="F30" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="H30" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="87" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="16" customFormat="1" ht="90">
-      <c r="A31" s="65">
-        <v>45786</v>
-      </c>
-      <c r="B31" s="66" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="67" t="s">
+      <c r="F31" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="D31" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="67" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="68" t="s">
+      <c r="G31" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="G31" s="67" t="s">
+      <c r="H31" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="I31" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="87" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="15" customFormat="1">
+      <c r="A32" s="58">
+        <v>45787</v>
+      </c>
+      <c r="B32" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="H31" s="67" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="88" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="15" customFormat="1" ht="60">
-      <c r="A32" s="58">
-        <v>45786</v>
-      </c>
-      <c r="B32" s="59" t="s">
+      <c r="C32" s="59" t="s">
         <v>143</v>
-      </c>
-      <c r="C32" s="60" t="s">
-        <v>144</v>
       </c>
       <c r="D32" s="60" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="60" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F32" s="61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G32" s="60" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H32" s="60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I32" s="60" t="s">
         <v>18</v>
       </c>
       <c r="J32" s="87" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="15" customFormat="1">
-      <c r="A33" s="58">
-        <v>45787</v>
-      </c>
-      <c r="B33" s="59" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" s="61" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="60" t="s">
-        <v>149</v>
-      </c>
-      <c r="H33" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="I33" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="87" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2550,10 +2512,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2566,27 +2528,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
@@ -2600,7 +2562,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D3" s="8">
         <v>45761</v>
@@ -2608,13 +2570,13 @@
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D4" s="11">
         <v>45761</v>
@@ -2622,13 +2584,13 @@
     </row>
     <row r="5" spans="1:4" ht="18.75">
       <c r="A5" s="9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D5" s="11">
         <v>45764</v>
@@ -2636,13 +2598,13 @@
     </row>
     <row r="6" spans="1:4" ht="18.75">
       <c r="A6" s="9" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D6" s="11">
         <v>45765</v>
@@ -2650,13 +2612,13 @@
     </row>
     <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D7" s="5">
         <v>45765</v>
@@ -2664,13 +2626,13 @@
     </row>
     <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D8" s="5">
         <v>45765</v>
@@ -2678,13 +2640,13 @@
     </row>
     <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D9" s="5">
         <v>45766</v>
@@ -2692,13 +2654,13 @@
     </row>
     <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D10" s="5">
         <v>45766</v>
@@ -2706,13 +2668,13 @@
     </row>
     <row r="11" spans="1:4" ht="18.75">
       <c r="A11" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D11" s="5">
         <v>45767</v>
@@ -2720,13 +2682,13 @@
     </row>
     <row r="12" spans="1:4" ht="18.75">
       <c r="A12" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D12" s="5">
         <v>45785</v>
@@ -2734,13 +2696,13 @@
     </row>
     <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D13" s="5">
         <v>45786</v>
@@ -2748,13 +2710,13 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D14" s="5">
         <v>45786</v>
@@ -2762,13 +2724,13 @@
     </row>
     <row r="15" spans="1:4" ht="18.75">
       <c r="A15" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="D15" s="5">
         <v>45786</v>
@@ -2776,13 +2738,13 @@
     </row>
     <row r="16" spans="1:4" ht="18.75">
       <c r="A16" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D16" s="5">
         <v>45786</v>
@@ -2790,13 +2752,13 @@
     </row>
     <row r="17" spans="1:4" ht="18.75">
       <c r="A17" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D17" s="5">
         <v>45786</v>
@@ -2804,13 +2766,13 @@
     </row>
     <row r="18" spans="1:4" ht="18.75">
       <c r="A18" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D18" s="5">
         <v>45786</v>
@@ -2818,13 +2780,13 @@
     </row>
     <row r="19" spans="1:4" ht="18.75">
       <c r="A19" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D19" s="5">
         <v>45786</v>
@@ -2832,13 +2794,13 @@
     </row>
     <row r="20" spans="1:4" ht="18.75">
       <c r="A20" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D20" s="5">
         <v>45787</v>
@@ -2846,13 +2808,13 @@
     </row>
     <row r="21" spans="1:4" ht="18.75">
       <c r="A21" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D21" s="5">
         <v>45787</v>
@@ -2860,13 +2822,13 @@
     </row>
     <row r="22" spans="1:4" ht="37.5">
       <c r="A22" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D22" s="5">
         <v>45787</v>
@@ -2874,15 +2836,29 @@
     </row>
     <row r="23" spans="1:4" ht="37.5">
       <c r="A23" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D23" s="5">
+        <v>45787</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="37.5">
+      <c r="A24" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="5">
         <v>45787</v>
       </c>
     </row>

</xml_diff>